<commit_message>
Added ammonia and GHSV filters
</commit_message>
<xml_diff>
--- a/TheKesselRun/Data/RAW/NH3_v4_Data.xlsx
+++ b/TheKesselRun/Data/RAW/NH3_v4_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23865" windowHeight="14040" tabRatio="738"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="23865" windowHeight="14040" tabRatio="738" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info 3" sheetId="6" r:id="rId1"/>
@@ -5899,7 +5899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -45620,8 +45620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45923,7 +45923,7 @@
         <v>103.8</v>
       </c>
       <c r="H13" s="69">
-        <v>1161.4000000000001</v>
+        <v>116.4</v>
       </c>
       <c r="I13" s="157">
         <v>9.1062510762872396E-3</v>

</xml_diff>

<commit_message>
Added some stuff for operator
</commit_message>
<xml_diff>
--- a/TheKesselRun/Data/RAW/NH3_v4_Data.xlsx
+++ b/TheKesselRun/Data/RAW/NH3_v4_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23865" windowHeight="14040" tabRatio="738" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="23865" windowHeight="14040" tabRatio="738" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info 3" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5013" uniqueCount="1564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5014" uniqueCount="1565">
   <si>
     <t>Sample</t>
   </si>
@@ -4619,9 +4619,6 @@
     <t>63 1312 RuScK</t>
   </si>
   <si>
-    <t>64 3112 RuScK</t>
-  </si>
-  <si>
     <t>rx7-2500</t>
   </si>
   <si>
@@ -4725,6 +4722,12 @@
   </si>
   <si>
     <t>36 12 K</t>
+  </si>
+  <si>
+    <t>64 3112 RuRhK</t>
+  </si>
+  <si>
+    <t>20 412 RuK</t>
   </si>
 </sst>
 </file>
@@ -6092,7 +6095,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F6" s="25">
         <v>0.2</v>
@@ -6128,7 +6131,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="F7" s="25">
         <v>0.2</v>
@@ -6412,7 +6415,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F15" s="25">
         <v>0.19900000000000001</v>
@@ -6444,7 +6447,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="F16" s="25">
         <v>0.2</v>
@@ -7243,16 +7246,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="115" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F1" s="115" t="s">
         <v>1535</v>
       </c>
-      <c r="F1" s="115" t="s">
+      <c r="J1" s="115" t="s">
         <v>1536</v>
       </c>
-      <c r="J1" s="115" t="s">
+      <c r="K1" s="115" t="s">
         <v>1537</v>
-      </c>
-      <c r="K1" s="115" t="s">
-        <v>1538</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -14225,19 +14228,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F1" t="s">
         <v>1535</v>
       </c>
-      <c r="F1" t="s">
-        <v>1536</v>
-      </c>
       <c r="I1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="J1" t="s">
         <v>1540</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1541</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1542</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -14265,7 +14268,7 @@
         <v>250</v>
       </c>
       <c r="H2" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I2">
         <f>AVERAGE(E2:E6)</f>
@@ -14555,7 +14558,7 @@
         <v>300</v>
       </c>
       <c r="H13" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I13" s="156">
         <f>AVERAGE(F13:F15)</f>
@@ -14720,7 +14723,7 @@
         <v>350</v>
       </c>
       <c r="H19" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I19" s="156">
         <f>AVERAGE(F19:F21)</f>
@@ -14981,7 +14984,7 @@
         <v>250</v>
       </c>
       <c r="H29" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I29" s="115">
         <f>AVERAGE(E29:E33)</f>
@@ -15313,7 +15316,7 @@
         <v>300</v>
       </c>
       <c r="H40" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I40" s="156">
         <f>AVERAGE(F40:F42)</f>
@@ -15499,7 +15502,7 @@
         <v>350</v>
       </c>
       <c r="H46" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I46" s="156">
         <f>AVERAGE(F46:F48)</f>
@@ -15792,7 +15795,7 @@
         <v>250</v>
       </c>
       <c r="H56" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I56" s="115">
         <f>AVERAGE(E56:E60)</f>
@@ -16124,7 +16127,7 @@
         <v>300</v>
       </c>
       <c r="H67" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I67" s="156">
         <f>AVERAGE(F67:F69)</f>
@@ -16310,7 +16313,7 @@
         <v>350</v>
       </c>
       <c r="H73" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I73" s="156">
         <f>AVERAGE(F73:F75)</f>
@@ -16603,7 +16606,7 @@
         <v>250</v>
       </c>
       <c r="H83" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I83" s="115">
         <f>AVERAGE(E83:E87)</f>
@@ -16935,7 +16938,7 @@
         <v>300</v>
       </c>
       <c r="H94" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I94" s="156">
         <f>AVERAGE(F94:F96)</f>
@@ -17121,7 +17124,7 @@
         <v>350</v>
       </c>
       <c r="H100" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I100" s="156">
         <f>AVERAGE(F100:F102)</f>
@@ -17414,7 +17417,7 @@
         <v>250</v>
       </c>
       <c r="H110" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I110" s="115">
         <f>AVERAGE(E110:E114)</f>
@@ -17746,7 +17749,7 @@
         <v>300</v>
       </c>
       <c r="H121" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I121" s="156">
         <f>AVERAGE(F121:F123)</f>
@@ -17932,7 +17935,7 @@
         <v>350</v>
       </c>
       <c r="H127" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I127" s="156">
         <f>AVERAGE(F127:F129)</f>
@@ -18225,7 +18228,7 @@
         <v>250</v>
       </c>
       <c r="H137" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I137" s="115">
         <f>AVERAGE(E137:E141)</f>
@@ -18557,7 +18560,7 @@
         <v>300</v>
       </c>
       <c r="H148" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I148" s="156">
         <f>AVERAGE(F148:F150)</f>
@@ -18743,7 +18746,7 @@
         <v>350</v>
       </c>
       <c r="H154" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I154" s="156">
         <f>AVERAGE(F154:F156)</f>
@@ -19036,7 +19039,7 @@
         <v>250</v>
       </c>
       <c r="H164" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I164" s="115">
         <f>AVERAGE(E164:E168)</f>
@@ -19368,7 +19371,7 @@
         <v>300</v>
       </c>
       <c r="H175" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I175" s="156">
         <f>AVERAGE(F175:F177)</f>
@@ -19554,7 +19557,7 @@
         <v>350</v>
       </c>
       <c r="H181" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I181" s="156">
         <f>AVERAGE(F181:F183)</f>
@@ -19847,7 +19850,7 @@
         <v>250</v>
       </c>
       <c r="H191" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I191" s="115">
         <f>AVERAGE(E191:E195)</f>
@@ -20179,7 +20182,7 @@
         <v>300</v>
       </c>
       <c r="H202" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I202" s="156">
         <f>AVERAGE(F202:F204)</f>
@@ -20365,7 +20368,7 @@
         <v>350</v>
       </c>
       <c r="H208" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I208" s="156">
         <f>AVERAGE(F208:F210)</f>
@@ -20658,7 +20661,7 @@
         <v>250</v>
       </c>
       <c r="H218" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I218" s="115">
         <f>AVERAGE(E218:E222)</f>
@@ -20990,7 +20993,7 @@
         <v>300</v>
       </c>
       <c r="H229" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I229" s="156">
         <f>AVERAGE(F229:F231)</f>
@@ -21176,7 +21179,7 @@
         <v>350</v>
       </c>
       <c r="H235" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I235" s="156">
         <f>AVERAGE(F235:F237)</f>
@@ -21653,7 +21656,7 @@
         <v>300</v>
       </c>
       <c r="H251" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I251" s="156">
         <f>AVERAGE(F251:F253)</f>
@@ -21839,7 +21842,7 @@
         <v>350</v>
       </c>
       <c r="H257" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I257" s="156">
         <f>AVERAGE(F257:F259)</f>
@@ -22132,7 +22135,7 @@
         <v>250</v>
       </c>
       <c r="H267" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I267" s="115">
         <f>AVERAGE(E267:E271)</f>
@@ -22464,7 +22467,7 @@
         <v>300</v>
       </c>
       <c r="H278" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I278" s="156">
         <f>AVERAGE(F278:F280)</f>
@@ -22650,7 +22653,7 @@
         <v>350</v>
       </c>
       <c r="H284" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I284" s="156">
         <f>AVERAGE(F284:F286)</f>
@@ -22943,7 +22946,7 @@
         <v>250</v>
       </c>
       <c r="H294" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I294" s="115">
         <f>AVERAGE(E294:E298)</f>
@@ -23275,7 +23278,7 @@
         <v>300</v>
       </c>
       <c r="H305" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I305" s="156">
         <f>AVERAGE(F305:F307)</f>
@@ -23461,7 +23464,7 @@
         <v>350</v>
       </c>
       <c r="H311" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I311" s="156">
         <f>AVERAGE(F311:F313)</f>
@@ -23754,7 +23757,7 @@
         <v>250</v>
       </c>
       <c r="H321" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I321" s="115">
         <f>AVERAGE(E321:E325)</f>
@@ -24086,7 +24089,7 @@
         <v>300</v>
       </c>
       <c r="H332" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I332" s="156">
         <f>AVERAGE(F332:F334)</f>
@@ -24272,7 +24275,7 @@
         <v>350</v>
       </c>
       <c r="H338" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I338" s="156">
         <f>AVERAGE(F338:F340)</f>
@@ -24565,7 +24568,7 @@
         <v>250</v>
       </c>
       <c r="H348" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I348" s="115">
         <f>AVERAGE(E348:E352)</f>
@@ -24896,7 +24899,7 @@
         <v>300</v>
       </c>
       <c r="H359" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I359" s="156">
         <f>AVERAGE(F359:F361)</f>
@@ -25082,7 +25085,7 @@
         <v>350</v>
       </c>
       <c r="H365" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I365" s="156">
         <f>AVERAGE(F365:F367)</f>
@@ -26339,19 +26342,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="115" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F1" s="115" t="s">
         <v>1535</v>
       </c>
-      <c r="F1" s="115" t="s">
-        <v>1536</v>
-      </c>
       <c r="I1" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="J1" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="K1" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -31948,8 +31951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32024,12 +32027,26 @@
       <c r="D3" s="100">
         <v>0</v>
       </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="96"/>
+      <c r="E3" s="93" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F3" s="95">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="136">
+        <v>104.2</v>
+      </c>
+      <c r="H3" s="136">
+        <v>93.04</v>
+      </c>
+      <c r="I3" s="95">
+        <f>100*((0.1*(G3-H3))/G3)</f>
+        <v>1.0710172744721687</v>
+      </c>
+      <c r="J3" s="137">
+        <f>G3/(F3/B$20)</f>
+        <v>2057.9500000000003</v>
+      </c>
       <c r="K3" s="103"/>
       <c r="L3" s="70"/>
       <c r="M3" s="74" t="s">
@@ -32297,7 +32314,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="93" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="F12" s="95">
         <v>0.20100000000000001</v>
@@ -32897,19 +32914,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F1" t="s">
         <v>1535</v>
       </c>
-      <c r="F1" t="s">
-        <v>1536</v>
-      </c>
       <c r="I1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1535</v>
+      </c>
+      <c r="K1" s="107" t="s">
         <v>1543</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1536</v>
-      </c>
-      <c r="K1" s="107" t="s">
-        <v>1544</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -32925,31 +32942,31 @@
       <c r="D2">
         <v>0.82640426914783904</v>
       </c>
-      <c r="E2" t="e">
+      <c r="E2">
         <f>('Info 5'!I$3-D2)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F2" s="155" t="e">
+        <v>0.22839314654834364</v>
+      </c>
+      <c r="F2" s="155">
         <f>E2</f>
-        <v>#DIV/0!</v>
+        <v>0.22839314654834364</v>
       </c>
       <c r="G2">
         <v>150</v>
       </c>
       <c r="H2" t="s">
-        <v>1539</v>
-      </c>
-      <c r="I2" t="e">
+        <v>1538</v>
+      </c>
+      <c r="I2">
         <f>AVERAGE(E2:E4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J2" t="e">
+        <v>0.24082163114684729</v>
+      </c>
+      <c r="J2">
         <f>I2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K2" s="107" t="e">
+        <v>0.24082163114684729</v>
+      </c>
+      <c r="K2" s="107">
         <f>_xlfn.STDEV.P(F2:F4)</f>
-        <v>#DIV/0!</v>
+        <v>8.8243927194999097E-3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -32965,13 +32982,13 @@
       <c r="D3">
         <v>0.805391252467762</v>
       </c>
-      <c r="E3" s="115" t="e">
+      <c r="E3" s="115">
         <f>('Info 5'!I$3-D3)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" s="155" t="e">
+        <v>0.24801282699694607</v>
+      </c>
+      <c r="F3" s="155">
         <f t="shared" ref="F3:F66" si="0">E3</f>
-        <v>#DIV/0!</v>
+        <v>0.24801282699694607</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -32987,13 +33004,13 @@
       <c r="D4">
         <v>0.80748392072638997</v>
       </c>
-      <c r="E4" s="115" t="e">
+      <c r="E4" s="115">
         <f>('Info 5'!I$3-D4)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" s="155" t="e">
+        <v>0.24605891989525219</v>
+      </c>
+      <c r="F4" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.24605891989525219</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -33009,31 +33026,31 @@
       <c r="D5">
         <v>0.53784885108639002</v>
       </c>
-      <c r="E5" s="115" t="e">
+      <c r="E5" s="115">
         <f>('Info 5'!I$3-D5)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="155" t="e">
+        <v>0.49781496162005506</v>
+      </c>
+      <c r="F5" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.49781496162005506</v>
       </c>
       <c r="G5">
         <v>250</v>
       </c>
       <c r="H5" t="s">
-        <v>1539</v>
-      </c>
-      <c r="I5" t="e">
+        <v>1538</v>
+      </c>
+      <c r="I5">
         <f>AVERAGE(E5:E7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J5" t="e">
+        <v>0.4909994149176824</v>
+      </c>
+      <c r="J5">
         <f>I5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K5" s="107" t="e">
+        <v>0.4909994149176824</v>
+      </c>
+      <c r="K5" s="107">
         <f>_xlfn.STDEV.P(F5:F7)</f>
-        <v>#DIV/0!</v>
+        <v>7.6704718155539732E-3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -33049,13 +33066,13 @@
       <c r="D6">
         <v>0.54097058015372002</v>
       </c>
-      <c r="E6" s="115" t="e">
+      <c r="E6" s="115">
         <f>('Info 5'!I$3-D6)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="155" t="e">
+        <v>0.49490022892457314</v>
+      </c>
+      <c r="F6" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.49490022892457314</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -33071,13 +33088,13 @@
       <c r="D7">
         <v>0.55662582677869898</v>
       </c>
-      <c r="E7" s="115" t="e">
+      <c r="E7" s="115">
         <f>('Info 5'!I$3-D7)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="155" t="e">
+        <v>0.48028305420841894</v>
+      </c>
+      <c r="F7" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.48028305420841894</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -33093,31 +33110,31 @@
       <c r="D8" s="2">
         <v>2.34880992630986E-2</v>
       </c>
-      <c r="E8" s="115" t="e">
+      <c r="E8" s="115">
         <f>('Info 5'!I$3-D8)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="155" t="e">
+        <v>0.97806935534753703</v>
+      </c>
+      <c r="F8" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.97806935534753703</v>
       </c>
       <c r="G8">
         <v>300</v>
       </c>
       <c r="H8" t="s">
-        <v>1539</v>
-      </c>
-      <c r="I8" t="e">
+        <v>1538</v>
+      </c>
+      <c r="I8">
         <f>AVERAGE(E8:E12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" t="e">
+        <v>0.98785535042637063</v>
+      </c>
+      <c r="J8">
         <f>I8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="107" t="e">
+        <v>0.98785535042637063</v>
+      </c>
+      <c r="K8" s="107">
         <f>_xlfn.STDEV.P(F8:F12)</f>
-        <v>#DIV/0!</v>
+        <v>7.8185564684575461E-3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -33133,13 +33150,13 @@
       <c r="D9" s="2">
         <v>2.0444639503584602E-2</v>
       </c>
-      <c r="E9" s="115" t="e">
+      <c r="E9" s="115">
         <f>('Info 5'!I$3-D9)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="155" t="e">
+        <v>0.98091100863554193</v>
+      </c>
+      <c r="F9" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.98091100863554193</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -33155,13 +33172,13 @@
       <c r="D10" s="2">
         <v>1.19988671941568E-2</v>
       </c>
-      <c r="E10" s="115" t="e">
+      <c r="E10" s="115">
         <f>('Info 5'!I$3-D10)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="155" t="e">
+        <v>0.98879675661620836</v>
+      </c>
+      <c r="F10" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.98879675661620836</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -33177,13 +33194,13 @@
       <c r="D11" s="2">
         <v>0</v>
       </c>
-      <c r="E11" s="115" t="e">
+      <c r="E11" s="115">
         <f>('Info 5'!I$3-D11)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F11" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -33199,13 +33216,13 @@
       <c r="D12" s="2">
         <v>9.1040414680006992E-3</v>
       </c>
-      <c r="E12" s="115" t="e">
+      <c r="E12" s="115">
         <f>('Info 5'!I$3-D12)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" s="155" t="e">
+        <v>0.99149963153256571</v>
+      </c>
+      <c r="F12" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.99149963153256571</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -33221,31 +33238,31 @@
       <c r="D13">
         <v>1.0078226667400001E-2</v>
       </c>
-      <c r="E13" s="115" t="e">
+      <c r="E13" s="115">
         <f>('Info 5'!I$3-D13)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="155" t="e">
+        <v>0.99059004284280394</v>
+      </c>
+      <c r="F13" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.99059004284280394</v>
       </c>
       <c r="G13">
         <v>400</v>
       </c>
       <c r="H13" t="s">
-        <v>1539</v>
-      </c>
-      <c r="I13" t="e">
+        <v>1538</v>
+      </c>
+      <c r="I13">
         <f>AVERAGE(E13:E15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" t="e">
+        <v>0.99037603779267813</v>
+      </c>
+      <c r="J13">
         <f>I13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K13" s="107" t="e">
+        <v>0.99037603779267813</v>
+      </c>
+      <c r="K13" s="107">
         <f>_xlfn.STDEV.P(F13:F15)</f>
-        <v>#DIV/0!</v>
+        <v>7.9467403482614656E-3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -33261,13 +33278,13 @@
       <c r="D14" s="2">
         <v>0</v>
       </c>
-      <c r="E14" s="115" t="e">
+      <c r="E14" s="115">
         <f>('Info 5'!I$3-D14)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F14" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -33283,13 +33300,13 @@
       <c r="D15" s="2">
         <v>2.08440626513276E-2</v>
       </c>
-      <c r="E15" s="115" t="e">
+      <c r="E15" s="115">
         <f>('Info 5'!I$3-D15)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="155" t="e">
+        <v>0.98053807053523001</v>
+      </c>
+      <c r="F15" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.98053807053523001</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -33305,28 +33322,28 @@
       <c r="D16">
         <v>0.51692085172648405</v>
       </c>
-      <c r="E16" s="115" t="e">
+      <c r="E16" s="115">
         <f>('Info 5'!I$3-D16)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="155" t="e">
+        <v>0.51735526209767335</v>
+      </c>
+      <c r="F16" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.51735526209767335</v>
       </c>
       <c r="G16">
         <v>250</v>
       </c>
-      <c r="I16" t="e">
+      <c r="I16">
         <f>AVERAGE(E16:E19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" t="e">
+        <v>0.51718237635790421</v>
+      </c>
+      <c r="J16">
         <f>I16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K16" s="107" t="e">
+        <v>0.51718237635790421</v>
+      </c>
+      <c r="K16" s="107">
         <f>_xlfn.STDEV.P(F16:F19)</f>
-        <v>#DIV/0!</v>
+        <v>8.6596344318960027E-3</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -33342,13 +33359,13 @@
       <c r="D17">
         <v>0.50959554567871301</v>
       </c>
-      <c r="E17" s="115" t="e">
+      <c r="E17" s="115">
         <f>('Info 5'!I$3-D17)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="155" t="e">
+        <v>0.52419483996664962</v>
+      </c>
+      <c r="F17" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.52419483996664962</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -33364,13 +33381,13 @@
       <c r="D18">
         <v>0.50959554567871301</v>
       </c>
-      <c r="E18" s="115" t="e">
+      <c r="E18" s="115">
         <f>('Info 5'!I$3-D18)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" s="155" t="e">
+        <v>0.52419483996664962</v>
+      </c>
+      <c r="F18" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.52419483996664962</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -33386,13 +33403,13 @@
       <c r="D19">
         <v>0.53231211827723701</v>
       </c>
-      <c r="E19" s="115" t="e">
+      <c r="E19" s="115">
         <f>('Info 5'!I$3-D19)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F19" s="155" t="e">
+        <v>0.50298456340064412</v>
+      </c>
+      <c r="F19" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.50298456340064412</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -33408,28 +33425,28 @@
       <c r="D20" s="2">
         <v>3.43154341459118E-3</v>
       </c>
-      <c r="E20" s="115" t="e">
+      <c r="E20" s="115">
         <f>('Info 5'!I$3-D20)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="155" t="e">
+        <v>0.99679599620250525</v>
+      </c>
+      <c r="F20" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.99679599620250525</v>
       </c>
       <c r="G20">
         <v>300</v>
       </c>
-      <c r="I20" t="e">
+      <c r="I20">
         <f>AVERAGE(E20:E22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" t="e">
+        <v>0.99761345675509772</v>
+      </c>
+      <c r="J20">
         <f>I20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="107" t="e">
+        <v>0.99761345675509772</v>
+      </c>
+      <c r="K20" s="107">
         <f>_xlfn.STDEV.P(F20:F22)</f>
-        <v>#DIV/0!</v>
+        <v>1.7152114456764689E-3</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -33445,13 +33462,13 @@
       <c r="D21" s="2">
         <v>0</v>
       </c>
-      <c r="E21" s="115" t="e">
+      <c r="E21" s="115">
         <f>('Info 5'!I$3-D21)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F21" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -33467,13 +33484,13 @@
       <c r="D22" s="2">
         <v>4.2365437101039597E-3</v>
       </c>
-      <c r="E22" s="115" t="e">
+      <c r="E22" s="115">
         <f>('Info 5'!I$3-D22)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" s="155" t="e">
+        <v>0.99604437406278823</v>
+      </c>
+      <c r="F22" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.99604437406278823</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -33489,28 +33506,28 @@
       <c r="D23" s="2">
         <v>2.11291843577389E-2</v>
       </c>
-      <c r="E23" s="115" t="e">
+      <c r="E23" s="115">
         <f>('Info 5'!I$3-D23)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F23" s="155" t="e">
+        <v>0.98027185474841949</v>
+      </c>
+      <c r="F23" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.98027185474841949</v>
       </c>
       <c r="G23">
         <v>350</v>
       </c>
-      <c r="I23" t="e">
+      <c r="I23">
         <f>AVERAGE(E23:E25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J23" t="e">
+        <v>0.99180714299499562</v>
+      </c>
+      <c r="J23">
         <f>I23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K23" s="107" t="e">
+        <v>0.99180714299499562</v>
+      </c>
+      <c r="K23" s="107">
         <f>_xlfn.STDEV.P(F23:F25)</f>
-        <v>#DIV/0!</v>
+        <v>8.3936012819425376E-3</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -33526,13 +33543,13 @@
       <c r="D24" s="2">
         <v>5.19488978118099E-3</v>
       </c>
-      <c r="E24" s="115" t="e">
+      <c r="E24" s="115">
         <f>('Info 5'!I$3-D24)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F24" s="155" t="e">
+        <v>0.99514957423656747</v>
+      </c>
+      <c r="F24" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.99514957423656747</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -33548,13 +33565,13 @@
       <c r="D25" s="2">
         <v>0</v>
       </c>
-      <c r="E25" s="115" t="e">
+      <c r="E25" s="115">
         <f>('Info 5'!I$3-D25)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F25" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -33570,28 +33587,28 @@
       <c r="D26" s="2">
         <v>5.4114071296246201E-3</v>
       </c>
-      <c r="E26" s="115" t="e">
+      <c r="E26" s="115">
         <f>('Info 5'!I$3-D26)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F26" s="155" t="e">
+        <v>0.99494741377323592</v>
+      </c>
+      <c r="F26" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.99494741377323592</v>
       </c>
       <c r="G26">
         <v>400</v>
       </c>
-      <c r="I26" t="e">
+      <c r="I26">
         <f>AVERAGE(E26:E28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J26" t="e">
+        <v>0.9983158045910786</v>
+      </c>
+      <c r="J26">
         <f>I26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K26" s="107" t="e">
+        <v>0.9983158045910786</v>
+      </c>
+      <c r="K26" s="107">
         <f>_xlfn.STDEV.P(F26:F28)</f>
-        <v>#DIV/0!</v>
+        <v>2.381811988983087E-3</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -33607,13 +33624,13 @@
       <c r="D27" s="2">
         <v>0</v>
       </c>
-      <c r="E27" s="115" t="e">
+      <c r="E27" s="115">
         <f>('Info 5'!I$3-D27)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F27" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F27" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -33629,13 +33646,13 @@
       <c r="D28" s="2">
         <v>0</v>
       </c>
-      <c r="E28" s="115" t="e">
+      <c r="E28" s="115">
         <f>('Info 5'!I$3-D28)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F28" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -33651,28 +33668,28 @@
       <c r="D29" s="2">
         <v>0</v>
       </c>
-      <c r="E29" s="115" t="e">
+      <c r="E29" s="115">
         <f>('Info 5'!I$3-D29)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F29" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F29" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>450</v>
       </c>
-      <c r="I29" t="e">
+      <c r="I29">
         <f>AVERAGE(E29:E31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J29" t="e">
+        <v>1</v>
+      </c>
+      <c r="J29">
         <f>I29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K29" s="107" t="e">
+        <v>1</v>
+      </c>
+      <c r="K29" s="107">
         <f>_xlfn.STDEV.P(F29:F31)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -33688,13 +33705,13 @@
       <c r="D30" s="2">
         <v>0</v>
       </c>
-      <c r="E30" s="115" t="e">
+      <c r="E30" s="115">
         <f>('Info 5'!I$3-D30)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F30" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F30" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -33710,13 +33727,13 @@
       <c r="D31" s="2">
         <v>0</v>
       </c>
-      <c r="E31" s="115" t="e">
+      <c r="E31" s="115">
         <f>('Info 5'!I$3-D31)/'Info 5'!I$3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F31" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F31" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -33758,7 +33775,7 @@
         <v>150</v>
       </c>
       <c r="H33" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I33" s="115" t="e">
         <f>AVERAGE(E33:E35)</f>
@@ -33850,7 +33867,7 @@
         <v>250</v>
       </c>
       <c r="H36" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I36" s="115" t="e">
         <f>AVERAGE(E36:E38)</f>
@@ -33942,7 +33959,7 @@
         <v>300</v>
       </c>
       <c r="H39" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I39" s="115" t="e">
         <f>AVERAGE(E39:E43)</f>
@@ -34086,7 +34103,7 @@
         <v>400</v>
       </c>
       <c r="H44" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I44" s="115" t="e">
         <f>AVERAGE(E44:E46)</f>
@@ -34668,7 +34685,7 @@
         <v>150</v>
       </c>
       <c r="H64" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I64" s="115" t="e">
         <f>AVERAGE(E64:E66)</f>
@@ -34760,7 +34777,7 @@
         <v>250</v>
       </c>
       <c r="H67" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I67" s="115" t="e">
         <f>AVERAGE(E67:E69)</f>
@@ -34852,7 +34869,7 @@
         <v>300</v>
       </c>
       <c r="H70" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I70" s="115" t="e">
         <f>AVERAGE(E70:E74)</f>
@@ -34996,7 +35013,7 @@
         <v>400</v>
       </c>
       <c r="H75" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I75" s="115" t="e">
         <f>AVERAGE(E75:E77)</f>
@@ -35578,7 +35595,7 @@
         <v>150</v>
       </c>
       <c r="H95" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I95" s="115" t="e">
         <f>AVERAGE(E95:E97)</f>
@@ -35670,7 +35687,7 @@
         <v>250</v>
       </c>
       <c r="H98" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I98" s="115" t="e">
         <f>AVERAGE(E98:E100)</f>
@@ -35762,7 +35779,7 @@
         <v>300</v>
       </c>
       <c r="H101" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I101" s="115" t="e">
         <f>AVERAGE(E101:E105)</f>
@@ -35906,7 +35923,7 @@
         <v>400</v>
       </c>
       <c r="H106" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I106" s="115" t="e">
         <f>AVERAGE(E106:E108)</f>
@@ -36488,7 +36505,7 @@
         <v>150</v>
       </c>
       <c r="H126" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I126" s="115" t="e">
         <f>AVERAGE(E126:E128)</f>
@@ -36580,7 +36597,7 @@
         <v>250</v>
       </c>
       <c r="H129" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I129" s="115" t="e">
         <f>AVERAGE(E129:E131)</f>
@@ -36672,7 +36689,7 @@
         <v>300</v>
       </c>
       <c r="H132" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I132" s="115" t="e">
         <f>AVERAGE(E132:E136)</f>
@@ -36816,7 +36833,7 @@
         <v>400</v>
       </c>
       <c r="H137" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I137" s="115" t="e">
         <f>AVERAGE(E137:E139)</f>
@@ -37398,7 +37415,7 @@
         <v>150</v>
       </c>
       <c r="H157" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I157" s="115">
         <f>AVERAGE(E157:E159)</f>
@@ -37490,7 +37507,7 @@
         <v>250</v>
       </c>
       <c r="H160" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I160" s="115">
         <f>AVERAGE(E160:E162)</f>
@@ -37582,7 +37599,7 @@
         <v>300</v>
       </c>
       <c r="H163" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I163" s="115">
         <f>AVERAGE(E163:E167)</f>
@@ -37726,7 +37743,7 @@
         <v>400</v>
       </c>
       <c r="H168" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I168" s="115">
         <f>AVERAGE(E168:E170)</f>
@@ -38308,7 +38325,7 @@
         <v>150</v>
       </c>
       <c r="H188" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I188" s="115">
         <f>AVERAGE(E188:E190)</f>
@@ -38400,7 +38417,7 @@
         <v>250</v>
       </c>
       <c r="H191" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I191" s="115">
         <f>AVERAGE(E191:E193)</f>
@@ -38492,7 +38509,7 @@
         <v>300</v>
       </c>
       <c r="H194" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I194" s="115">
         <f>AVERAGE(E194:E198)</f>
@@ -38636,7 +38653,7 @@
         <v>400</v>
       </c>
       <c r="H199" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I199" s="115">
         <f>AVERAGE(E199:E201)</f>
@@ -39226,7 +39243,7 @@
         <v>150</v>
       </c>
       <c r="H219" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I219" s="115">
         <f>AVERAGE(E219:E221)</f>
@@ -39318,7 +39335,7 @@
         <v>250</v>
       </c>
       <c r="H222" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I222" s="115">
         <f>AVERAGE(E222:E224)</f>
@@ -39410,7 +39427,7 @@
         <v>300</v>
       </c>
       <c r="H225" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I225" s="115">
         <f>AVERAGE(E225:E229)</f>
@@ -39554,7 +39571,7 @@
         <v>400</v>
       </c>
       <c r="H230" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I230" s="115">
         <f>AVERAGE(E230:E232)</f>
@@ -40144,7 +40161,7 @@
         <v>150</v>
       </c>
       <c r="H250" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I250" s="115">
         <f>AVERAGE(E250:E252)</f>
@@ -40236,7 +40253,7 @@
         <v>250</v>
       </c>
       <c r="H253" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I253" s="115">
         <f>AVERAGE(E253:E255)</f>
@@ -40328,7 +40345,7 @@
         <v>300</v>
       </c>
       <c r="H256" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I256" s="115">
         <f>AVERAGE(E256:E260)</f>
@@ -40472,7 +40489,7 @@
         <v>400</v>
       </c>
       <c r="H261" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I261" s="115">
         <f>AVERAGE(E261:E263)</f>
@@ -41062,7 +41079,7 @@
         <v>150</v>
       </c>
       <c r="H281" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I281" s="115">
         <f>AVERAGE(E281:E283)</f>
@@ -41154,7 +41171,7 @@
         <v>250</v>
       </c>
       <c r="H284" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I284" s="115">
         <f>AVERAGE(E284:E286)</f>
@@ -41246,7 +41263,7 @@
         <v>300</v>
       </c>
       <c r="H287" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I287" s="115">
         <f>AVERAGE(E287:E291)</f>
@@ -41390,7 +41407,7 @@
         <v>400</v>
       </c>
       <c r="H292" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I292" s="115">
         <f>AVERAGE(E292:E294)</f>
@@ -41980,7 +41997,7 @@
         <v>150</v>
       </c>
       <c r="H312" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I312" s="115">
         <f>AVERAGE(E312:E314)</f>
@@ -42072,7 +42089,7 @@
         <v>250</v>
       </c>
       <c r="H315" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I315" s="115">
         <f>AVERAGE(E315:E317)</f>
@@ -42164,7 +42181,7 @@
         <v>300</v>
       </c>
       <c r="H318" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I318" s="115">
         <f>AVERAGE(E318:E322)</f>
@@ -42308,7 +42325,7 @@
         <v>400</v>
       </c>
       <c r="H323" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I323" s="115">
         <f>AVERAGE(E323:E325)</f>
@@ -42898,7 +42915,7 @@
         <v>150</v>
       </c>
       <c r="H343" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I343" s="115">
         <f>AVERAGE(E343:E345)</f>
@@ -42990,7 +43007,7 @@
         <v>250</v>
       </c>
       <c r="H346" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I346" s="115">
         <f>AVERAGE(E346:E348)</f>
@@ -43082,7 +43099,7 @@
         <v>300</v>
       </c>
       <c r="H349" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I349" s="115">
         <f>AVERAGE(E349:E353)</f>
@@ -43226,7 +43243,7 @@
         <v>400</v>
       </c>
       <c r="H354" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I354" s="115">
         <f>AVERAGE(E354:E356)</f>
@@ -43816,7 +43833,7 @@
         <v>150</v>
       </c>
       <c r="H374" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I374" s="115">
         <f>AVERAGE(E374:E376)</f>
@@ -43908,7 +43925,7 @@
         <v>250</v>
       </c>
       <c r="H377" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I377" s="115">
         <f>AVERAGE(E377:E379)</f>
@@ -44000,7 +44017,7 @@
         <v>300</v>
       </c>
       <c r="H380" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I380" s="115">
         <f>AVERAGE(E380:E384)</f>
@@ -44144,7 +44161,7 @@
         <v>400</v>
       </c>
       <c r="H385" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I385" s="115">
         <f>AVERAGE(E385:E387)</f>
@@ -44734,7 +44751,7 @@
         <v>150</v>
       </c>
       <c r="H405" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I405" s="115">
         <f>AVERAGE(E405:E407)</f>
@@ -44826,7 +44843,7 @@
         <v>250</v>
       </c>
       <c r="H408" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I408" s="115">
         <f>AVERAGE(E408:E410)</f>
@@ -44918,7 +44935,7 @@
         <v>300</v>
       </c>
       <c r="H411" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I411" s="115">
         <f>AVERAGE(E411:E415)</f>
@@ -45062,7 +45079,7 @@
         <v>400</v>
       </c>
       <c r="H416" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I416" s="115">
         <f>AVERAGE(E416:E418)</f>
@@ -45620,7 +45637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -45663,7 +45680,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="F3" s="69">
         <v>0.2</v>
@@ -45690,7 +45707,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="69" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="F4" s="69">
         <v>0.2</v>
@@ -45740,7 +45757,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="69" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="F6" s="69">
         <v>0.20300000000000001</v>
@@ -45766,7 +45783,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="69" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="F7" s="69">
         <v>0.20399999999999999</v>
@@ -45792,7 +45809,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="69" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F8" s="69">
         <v>0.2</v>
@@ -45818,7 +45835,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="69" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="F9" s="69">
         <v>0.2</v>
@@ -45844,7 +45861,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="69" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="F10" s="69">
         <v>0.20200000000000001</v>
@@ -45888,7 +45905,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="69" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="F12" s="69">
         <v>0.20200000000000001</v>
@@ -45914,7 +45931,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="69" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="F13" s="69">
         <v>0.19900000000000001</v>
@@ -46393,19 +46410,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="115" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F1" s="115" t="s">
         <v>1535</v>
       </c>
-      <c r="F1" s="115" t="s">
-        <v>1536</v>
-      </c>
       <c r="I1" s="115" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="J1" s="115" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="K1" s="115" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="M1" s="115" t="s">
         <v>1395</v>
@@ -46439,7 +46456,7 @@
         <v>300</v>
       </c>
       <c r="H2" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I2" s="161" t="e">
         <f>AVERAGE(E2:E3)</f>
@@ -46485,7 +46502,7 @@
         <v>300</v>
       </c>
       <c r="H3" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="M3" s="115">
         <v>1</v>
@@ -46519,7 +46536,7 @@
         <v>350</v>
       </c>
       <c r="H4" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I4" s="115" t="e">
         <f>AVERAGE(E4:E6)</f>
@@ -46565,7 +46582,7 @@
         <v>350</v>
       </c>
       <c r="H5" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="M5" s="115">
         <v>3</v>
@@ -46599,7 +46616,7 @@
         <v>350</v>
       </c>
       <c r="H6" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="M6" s="115">
         <v>4</v>
@@ -46633,7 +46650,7 @@
         <v>400</v>
       </c>
       <c r="H7" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I7" s="161" t="e">
         <f>AVERAGE(E7:E9)</f>
@@ -46679,7 +46696,7 @@
         <v>400</v>
       </c>
       <c r="H8" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="M8" s="115">
         <v>6</v>
@@ -46713,7 +46730,7 @@
         <v>400</v>
       </c>
       <c r="H9" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="M9" s="115">
         <v>7</v>
@@ -47124,7 +47141,7 @@
         <v>300</v>
       </c>
       <c r="H21" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I21" s="161">
         <f>AVERAGE(E21:E22)</f>
@@ -47163,7 +47180,7 @@
         <v>300</v>
       </c>
       <c r="H22" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -47191,7 +47208,7 @@
         <v>350</v>
       </c>
       <c r="H23" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I23" s="115" t="e">
         <f>AVERAGE(E23:E25)</f>
@@ -47230,7 +47247,7 @@
         <v>350</v>
       </c>
       <c r="H24" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -47257,7 +47274,7 @@
         <v>350</v>
       </c>
       <c r="H25" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -47285,7 +47302,7 @@
         <v>400</v>
       </c>
       <c r="H26" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I26" s="161" t="e">
         <f>AVERAGE(E26:E28)</f>
@@ -47325,7 +47342,7 @@
         <v>400</v>
       </c>
       <c r="H27" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -47353,7 +47370,7 @@
         <v>400</v>
       </c>
       <c r="H28" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -47699,7 +47716,7 @@
         <v>300</v>
       </c>
       <c r="H40" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I40" s="161" t="e">
         <f>AVERAGE(E40:E41)</f>
@@ -47739,7 +47756,7 @@
         <v>300</v>
       </c>
       <c r="H41" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -47767,7 +47784,7 @@
         <v>350</v>
       </c>
       <c r="H42" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I42" s="115" t="e">
         <f>AVERAGE(E42:E44)</f>
@@ -47807,7 +47824,7 @@
         <v>350</v>
       </c>
       <c r="H43" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -47835,7 +47852,7 @@
         <v>350</v>
       </c>
       <c r="H44" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -47863,7 +47880,7 @@
         <v>400</v>
       </c>
       <c r="H45" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I45" s="161" t="e">
         <f>AVERAGE(E45:E47)</f>
@@ -47903,7 +47920,7 @@
         <v>400</v>
       </c>
       <c r="H46" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -47931,7 +47948,7 @@
         <v>400</v>
       </c>
       <c r="H47" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -48282,7 +48299,7 @@
         <v>300</v>
       </c>
       <c r="H59" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I59" s="161" t="e">
         <f>AVERAGE(E59:E60)</f>
@@ -48322,7 +48339,7 @@
         <v>300</v>
       </c>
       <c r="H60" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -48350,7 +48367,7 @@
         <v>350</v>
       </c>
       <c r="H61" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I61" s="115" t="e">
         <f>AVERAGE(E61:E63)</f>
@@ -48390,7 +48407,7 @@
         <v>350</v>
       </c>
       <c r="H62" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -48418,7 +48435,7 @@
         <v>350</v>
       </c>
       <c r="H63" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -48446,7 +48463,7 @@
         <v>400</v>
       </c>
       <c r="H64" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I64" s="161" t="e">
         <f>AVERAGE(E64:E66)</f>
@@ -48486,7 +48503,7 @@
         <v>400</v>
       </c>
       <c r="H65" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -48514,7 +48531,7 @@
         <v>400</v>
       </c>
       <c r="H66" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -48865,7 +48882,7 @@
         <v>300</v>
       </c>
       <c r="H78" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I78" s="161" t="e">
         <f>AVERAGE(E78:E79)</f>
@@ -48905,7 +48922,7 @@
         <v>300</v>
       </c>
       <c r="H79" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -48933,7 +48950,7 @@
         <v>350</v>
       </c>
       <c r="H80" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I80" s="115" t="e">
         <f>AVERAGE(E80:E82)</f>
@@ -48973,7 +48990,7 @@
         <v>350</v>
       </c>
       <c r="H81" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -49001,7 +49018,7 @@
         <v>350</v>
       </c>
       <c r="H82" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -49029,7 +49046,7 @@
         <v>400</v>
       </c>
       <c r="H83" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I83" s="161" t="e">
         <f>AVERAGE(E83:E85)</f>
@@ -49069,7 +49086,7 @@
         <v>400</v>
       </c>
       <c r="H84" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -49097,7 +49114,7 @@
         <v>400</v>
       </c>
       <c r="H85" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -49448,7 +49465,7 @@
         <v>300</v>
       </c>
       <c r="H97" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I97" s="161" t="e">
         <f>AVERAGE(E97:E98)</f>
@@ -49488,7 +49505,7 @@
         <v>300</v>
       </c>
       <c r="H98" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -49516,7 +49533,7 @@
         <v>350</v>
       </c>
       <c r="H99" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I99" s="115" t="e">
         <f>AVERAGE(E99:E101)</f>
@@ -49556,7 +49573,7 @@
         <v>350</v>
       </c>
       <c r="H100" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -49584,7 +49601,7 @@
         <v>350</v>
       </c>
       <c r="H101" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -49612,7 +49629,7 @@
         <v>400</v>
       </c>
       <c r="H102" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I102" s="161" t="e">
         <f>AVERAGE(E102:E104)</f>
@@ -49652,7 +49669,7 @@
         <v>400</v>
       </c>
       <c r="H103" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -49680,7 +49697,7 @@
         <v>400</v>
       </c>
       <c r="H104" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -50031,7 +50048,7 @@
         <v>300</v>
       </c>
       <c r="H116" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I116" s="161" t="e">
         <f>AVERAGE(E116:E117)</f>
@@ -50071,7 +50088,7 @@
         <v>300</v>
       </c>
       <c r="H117" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
@@ -50099,7 +50116,7 @@
         <v>350</v>
       </c>
       <c r="H118" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I118" s="115" t="e">
         <f>AVERAGE(E118:E120)</f>
@@ -50139,7 +50156,7 @@
         <v>350</v>
       </c>
       <c r="H119" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -50167,7 +50184,7 @@
         <v>350</v>
       </c>
       <c r="H120" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -50195,7 +50212,7 @@
         <v>400</v>
       </c>
       <c r="H121" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I121" s="161" t="e">
         <f>AVERAGE(E121:E123)</f>
@@ -50235,7 +50252,7 @@
         <v>400</v>
       </c>
       <c r="H122" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -50263,7 +50280,7 @@
         <v>400</v>
       </c>
       <c r="H123" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -50621,7 +50638,7 @@
         <v>300</v>
       </c>
       <c r="H135" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I135" s="161" t="e">
         <f>AVERAGE(E135:E136)</f>
@@ -50661,7 +50678,7 @@
         <v>300</v>
       </c>
       <c r="H136" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
@@ -50689,7 +50706,7 @@
         <v>350</v>
       </c>
       <c r="H137" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I137" s="115" t="e">
         <f>AVERAGE(E137:E139)</f>
@@ -50729,7 +50746,7 @@
         <v>350</v>
       </c>
       <c r="H138" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
@@ -50757,7 +50774,7 @@
         <v>350</v>
       </c>
       <c r="H139" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
@@ -50785,7 +50802,7 @@
         <v>400</v>
       </c>
       <c r="H140" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I140" s="161" t="e">
         <f>AVERAGE(E140:E142)</f>
@@ -50825,7 +50842,7 @@
         <v>400</v>
       </c>
       <c r="H141" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
@@ -50853,7 +50870,7 @@
         <v>400</v>
       </c>
       <c r="H142" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
@@ -51207,7 +51224,7 @@
         <v>300</v>
       </c>
       <c r="H154" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I154" s="161" t="e">
         <f>AVERAGE(E154:E155)</f>
@@ -51247,7 +51264,7 @@
         <v>300</v>
       </c>
       <c r="H155" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
@@ -51275,7 +51292,7 @@
         <v>350</v>
       </c>
       <c r="H156" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I156" s="115" t="e">
         <f>AVERAGE(E156:E158)</f>
@@ -51315,7 +51332,7 @@
         <v>350</v>
       </c>
       <c r="H157" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
@@ -51343,7 +51360,7 @@
         <v>350</v>
       </c>
       <c r="H158" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
@@ -51371,7 +51388,7 @@
         <v>400</v>
       </c>
       <c r="H159" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I159" s="161" t="e">
         <f>AVERAGE(E159:E161)</f>
@@ -51411,7 +51428,7 @@
         <v>400</v>
       </c>
       <c r="H160" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
@@ -51439,7 +51456,7 @@
         <v>400</v>
       </c>
       <c r="H161" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
@@ -51801,7 +51818,7 @@
         <v>300</v>
       </c>
       <c r="H174" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I174" s="161" t="e">
         <f>AVERAGE(E174:E175)</f>
@@ -51841,7 +51858,7 @@
         <v>300</v>
       </c>
       <c r="H175" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
@@ -51869,7 +51886,7 @@
         <v>350</v>
       </c>
       <c r="H176" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I176" s="115" t="e">
         <f>AVERAGE(E176:E178)</f>
@@ -51909,7 +51926,7 @@
         <v>350</v>
       </c>
       <c r="H177" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
@@ -51937,7 +51954,7 @@
         <v>350</v>
       </c>
       <c r="H178" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
@@ -51965,7 +51982,7 @@
         <v>400</v>
       </c>
       <c r="H179" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I179" s="161" t="e">
         <f>AVERAGE(E179:E181)</f>
@@ -52005,7 +52022,7 @@
         <v>400</v>
       </c>
       <c r="H180" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
@@ -52033,7 +52050,7 @@
         <v>400</v>
       </c>
       <c r="H181" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
@@ -52391,7 +52408,7 @@
         <v>300</v>
       </c>
       <c r="H193" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I193" s="161" t="e">
         <f>AVERAGE(E193:E194)</f>
@@ -52431,7 +52448,7 @@
         <v>300</v>
       </c>
       <c r="H194" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
@@ -52459,7 +52476,7 @@
         <v>350</v>
       </c>
       <c r="H195" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I195" s="115" t="e">
         <f>AVERAGE(E195:E197)</f>
@@ -52499,7 +52516,7 @@
         <v>350</v>
       </c>
       <c r="H196" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
@@ -52527,7 +52544,7 @@
         <v>350</v>
       </c>
       <c r="H197" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
@@ -52555,7 +52572,7 @@
         <v>400</v>
       </c>
       <c r="H198" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I198" s="161" t="e">
         <f>AVERAGE(E198:E200)</f>
@@ -52595,7 +52612,7 @@
         <v>400</v>
       </c>
       <c r="H199" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
@@ -52623,7 +52640,7 @@
         <v>400</v>
       </c>
       <c r="H200" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
@@ -52920,7 +52937,7 @@
         <v>300</v>
       </c>
       <c r="H213" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I213" s="161" t="e">
         <f>AVERAGE(E213:E214)</f>
@@ -52960,7 +52977,7 @@
         <v>300</v>
       </c>
       <c r="H214" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
@@ -52988,7 +53005,7 @@
         <v>350</v>
       </c>
       <c r="H215" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I215" s="115" t="e">
         <f>AVERAGE(E215:E217)</f>
@@ -53028,7 +53045,7 @@
         <v>350</v>
       </c>
       <c r="H216" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
@@ -53056,7 +53073,7 @@
         <v>350</v>
       </c>
       <c r="H217" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
@@ -53084,7 +53101,7 @@
         <v>400</v>
       </c>
       <c r="H218" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I218" s="161" t="e">
         <f>AVERAGE(E218:E220)</f>
@@ -53124,7 +53141,7 @@
         <v>400</v>
       </c>
       <c r="H219" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
@@ -53152,7 +53169,7 @@
         <v>400</v>
       </c>
       <c r="H220" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
@@ -53506,7 +53523,7 @@
         <v>300</v>
       </c>
       <c r="H233" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I233" s="161" t="e">
         <f>AVERAGE(E233:E234)</f>
@@ -53546,7 +53563,7 @@
         <v>300</v>
       </c>
       <c r="H234" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
@@ -53574,7 +53591,7 @@
         <v>350</v>
       </c>
       <c r="H235" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I235" s="115" t="e">
         <f>AVERAGE(E235:E237)</f>
@@ -53614,7 +53631,7 @@
         <v>350</v>
       </c>
       <c r="H236" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
@@ -53642,7 +53659,7 @@
         <v>350</v>
       </c>
       <c r="H237" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
@@ -53670,7 +53687,7 @@
         <v>400</v>
       </c>
       <c r="H238" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I238" s="161" t="e">
         <f>AVERAGE(E238:E240)</f>
@@ -53710,7 +53727,7 @@
         <v>400</v>
       </c>
       <c r="H239" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
@@ -53738,7 +53755,7 @@
         <v>400</v>
       </c>
       <c r="H240" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.25">
@@ -54096,7 +54113,7 @@
         <v>300</v>
       </c>
       <c r="H252" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I252" s="161" t="e">
         <f>AVERAGE(E252:E253)</f>
@@ -54136,7 +54153,7 @@
         <v>300</v>
       </c>
       <c r="H253" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="254" spans="1:11" x14ac:dyDescent="0.25">
@@ -54164,7 +54181,7 @@
         <v>350</v>
       </c>
       <c r="H254" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I254" s="115" t="e">
         <f>AVERAGE(E254:E256)</f>
@@ -54204,7 +54221,7 @@
         <v>350</v>
       </c>
       <c r="H255" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.25">
@@ -54232,7 +54249,7 @@
         <v>350</v>
       </c>
       <c r="H256" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.25">
@@ -54260,7 +54277,7 @@
         <v>400</v>
       </c>
       <c r="H257" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="I257" s="161" t="e">
         <f>AVERAGE(E257:E259)</f>
@@ -54300,7 +54317,7 @@
         <v>400</v>
       </c>
       <c r="H258" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.25">
@@ -54328,7 +54345,7 @@
         <v>400</v>
       </c>
       <c r="H259" s="115" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.25">
@@ -55069,7 +55086,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55306,7 +55323,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="135" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F7" s="136">
         <v>0.19853000000000001</v>
@@ -55345,7 +55362,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="135" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="F8" s="136">
         <v>0.19864999999999999</v>
@@ -55378,7 +55395,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="135" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="F9" s="136">
         <v>0.19986999999999999</v>
@@ -55411,7 +55428,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="135" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="F10" s="136">
         <v>0.19900999999999999</v>
@@ -55479,7 +55496,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="135" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="F12" s="136">
         <v>0.19954</v>
@@ -55629,7 +55646,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="135" t="s">
-        <v>1528</v>
+        <v>1563</v>
       </c>
       <c r="F16" s="136">
         <v>0.19903000000000001</v>
@@ -55825,7 +55842,7 @@
       <c r="B23" s="115"/>
       <c r="C23" s="115"/>
       <c r="D23" s="117" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E23" s="129"/>
       <c r="F23" s="117" t="s">
@@ -55850,7 +55867,7 @@
       <c r="B24" s="115"/>
       <c r="C24" s="115"/>
       <c r="D24" s="117" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="E24" s="129" t="s">
         <v>1440</v>
@@ -55900,7 +55917,7 @@
       <c r="B26" s="115"/>
       <c r="C26" s="115"/>
       <c r="D26" s="117" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="E26" s="129" t="s">
         <v>1442</v>
@@ -55952,7 +55969,7 @@
       <c r="B28" s="115"/>
       <c r="C28" s="115"/>
       <c r="D28" s="117" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="E28" s="117" t="s">
         <v>1445</v>
@@ -55971,7 +55988,7 @@
         <v>1412</v>
       </c>
       <c r="M28" s="115" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="N28" s="115"/>
       <c r="O28" s="115">
@@ -56010,7 +56027,7 @@
       <c r="B30" s="115"/>
       <c r="C30" s="115"/>
       <c r="D30" s="117" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="E30" s="117" t="s">
         <v>1447</v>

</xml_diff>

<commit_message>
Code changes reflecting rework Fixed minor bugs Reran some code for Katie
</commit_message>
<xml_diff>
--- a/TheKesselRun/Data/RAW/NH3_v4_Data.xlsx
+++ b/TheKesselRun/Data/RAW/NH3_v4_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quick\PycharmProjects\CatalystExMachina\TheKesselRun\Data\RAW\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCC152F-0F5F-43A5-AB2B-8D9350C46453}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23865" windowHeight="14040" tabRatio="738" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="23865" windowHeight="14040" tabRatio="738" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info 3" sheetId="6" r:id="rId1"/>
@@ -23,8 +24,13 @@
     <sheet name="Info 7" sheetId="10" r:id="rId9"/>
     <sheet name="RXN 7" sheetId="5" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5014" uniqueCount="1565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5021" uniqueCount="1572">
   <si>
     <t>Sample</t>
   </si>
@@ -4728,12 +4734,33 @@
   </si>
   <si>
     <t>20 412 RuK</t>
+  </si>
+  <si>
+    <t>24 412 RuK</t>
+  </si>
+  <si>
+    <t>21 412 RuK</t>
+  </si>
+  <si>
+    <t>22 412 RuK</t>
+  </si>
+  <si>
+    <t>RuK 5ml</t>
+  </si>
+  <si>
+    <t>RuK 6ml</t>
+  </si>
+  <si>
+    <t>RuK 8ml</t>
+  </si>
+  <si>
+    <t>RuK 20ml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -5043,7 +5070,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5479,6 +5506,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="118">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -5689,6 +5719,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5724,6 +5771,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5899,7 +5963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7214,7 +7278,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14199,7 +14263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K373"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25350,7 +25414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26313,7 +26377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K414"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -31948,11 +32012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31960,7 +32024,7 @@
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="70"/>
       <c r="B1" s="70"/>
       <c r="C1" s="70"/>
@@ -31980,7 +32044,7 @@
       <c r="O1" s="70"/>
       <c r="P1" s="70"/>
     </row>
-    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="70" t="s">
         <v>1394</v>
       </c>
@@ -32018,7 +32082,7 @@
       <c r="O2" s="168"/>
       <c r="P2" s="168"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="73">
         <v>43135</v>
       </c>
@@ -32061,20 +32125,37 @@
       <c r="P3" s="76" t="s">
         <v>1407</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S3" s="173" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="73"/>
       <c r="B4" s="70"/>
       <c r="C4" s="70"/>
       <c r="D4" s="100">
         <v>1</v>
       </c>
-      <c r="E4" s="93"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="96"/>
+      <c r="E4" s="135" t="s">
+        <v>1566</v>
+      </c>
+      <c r="F4" s="95">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="G4" s="136">
+        <v>110.6</v>
+      </c>
+      <c r="H4" s="136">
+        <v>99.89</v>
+      </c>
+      <c r="I4" s="95">
+        <f t="shared" ref="I4:I5" si="0">100*((0.1*(G4-H4))/G4)</f>
+        <v>0.96835443037974656</v>
+      </c>
+      <c r="J4" s="137">
+        <f t="shared" ref="J4:J5" si="1">G4/(F4/B$20)</f>
+        <v>2162.7227722772277</v>
+      </c>
       <c r="K4" s="103"/>
       <c r="L4" s="70"/>
       <c r="M4" s="77">
@@ -32087,20 +32168,37 @@
         <v>1460</v>
       </c>
       <c r="P4" s="170"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="70"/>
       <c r="B5" s="70"/>
       <c r="C5" s="70"/>
       <c r="D5" s="100">
         <v>2</v>
       </c>
-      <c r="E5" s="93"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="96"/>
+      <c r="E5" s="135" t="s">
+        <v>1567</v>
+      </c>
+      <c r="F5" s="95">
+        <v>0.158</v>
+      </c>
+      <c r="G5" s="136">
+        <v>111.5</v>
+      </c>
+      <c r="H5" s="136">
+        <v>100.6</v>
+      </c>
+      <c r="I5" s="95">
+        <f t="shared" si="0"/>
+        <v>0.97757847533632336</v>
+      </c>
+      <c r="J5" s="137">
+        <f t="shared" si="1"/>
+        <v>2787.5</v>
+      </c>
       <c r="K5" s="103"/>
       <c r="L5" s="70"/>
       <c r="M5" s="77">
@@ -32113,8 +32211,11 @@
         <v>1409</v>
       </c>
       <c r="P5" s="171"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="70"/>
       <c r="B6" s="70"/>
       <c r="C6" s="70"/>
@@ -32138,19 +32239,33 @@
         <v>470</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="70"/>
       <c r="B7" s="97"/>
       <c r="C7" s="97"/>
       <c r="D7" s="98">
         <v>4</v>
       </c>
-      <c r="E7" s="93"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="96"/>
+      <c r="E7" s="135" t="s">
+        <v>1565</v>
+      </c>
+      <c r="F7" s="95">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="G7" s="136">
+        <v>97.61</v>
+      </c>
+      <c r="H7" s="136">
+        <v>87.74</v>
+      </c>
+      <c r="I7" s="95">
+        <f t="shared" ref="I7" si="2">100*((0.1*(G7-H7))/G7)</f>
+        <v>1.0111668886384597</v>
+      </c>
+      <c r="J7" s="137">
+        <f t="shared" ref="J7" si="3">G7/(F7/B$20)</f>
+        <v>1937.4849246231156</v>
+      </c>
       <c r="K7" s="103"/>
       <c r="L7" s="70" t="s">
         <v>1413</v>
@@ -32161,8 +32276,11 @@
       <c r="P7" s="81">
         <v>450</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="70"/>
       <c r="B8" s="97"/>
       <c r="C8" s="97"/>
@@ -32198,7 +32316,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="70"/>
       <c r="B9" s="97"/>
       <c r="C9" s="97"/>
@@ -32234,7 +32352,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="70"/>
       <c r="B10" s="97"/>
       <c r="C10" s="97"/>
@@ -32270,7 +32388,7 @@
       <c r="O10" s="171"/>
       <c r="P10" s="171"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="70"/>
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
@@ -32306,7 +32424,7 @@
       <c r="O11" s="171"/>
       <c r="P11" s="171"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="70"/>
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
@@ -32338,7 +32456,7 @@
       <c r="O12" s="72"/>
       <c r="P12" s="72"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="70"/>
       <c r="B13" s="70"/>
       <c r="C13" s="70"/>
@@ -32370,7 +32488,7 @@
       <c r="O13" s="72"/>
       <c r="P13" s="72"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="70"/>
       <c r="B14" s="70"/>
       <c r="C14" s="70"/>
@@ -32402,7 +32520,7 @@
       <c r="O14" s="72"/>
       <c r="P14" s="72"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="70"/>
       <c r="B15" s="70"/>
       <c r="C15" s="70"/>
@@ -32434,7 +32552,7 @@
       <c r="O15" s="72"/>
       <c r="P15" s="72"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="70"/>
       <c r="B16" s="70"/>
       <c r="C16" s="70"/>
@@ -32886,7 +33004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K434"/>
   <sheetViews>
     <sheetView topLeftCell="A319" workbookViewId="0">
@@ -33763,13 +33881,13 @@
       <c r="D33">
         <v>0.84501980587879399</v>
       </c>
-      <c r="E33" s="115" t="e">
+      <c r="E33" s="115">
         <f>('Info 5'!I$4-D33)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F33" s="155" t="e">
+        <v>0.12736516778529744</v>
+      </c>
+      <c r="F33" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.12736516778529744</v>
       </c>
       <c r="G33" s="115">
         <v>150</v>
@@ -33777,17 +33895,17 @@
       <c r="H33" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I33" s="115" t="e">
+      <c r="I33" s="115">
         <f>AVERAGE(E33:E35)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J33" s="115" t="e">
+        <v>0.15065084781991178</v>
+      </c>
+      <c r="J33" s="115">
         <f>I33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K33" s="107" t="e">
+        <v>0.15065084781991178</v>
+      </c>
+      <c r="K33" s="107">
         <f>_xlfn.STDEV.P(F33:F35)</f>
-        <v>#DIV/0!</v>
+        <v>1.7787345897674667E-2</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -33803,13 +33921,13 @@
       <c r="D34">
         <v>0.81917701907894103</v>
       </c>
-      <c r="E34" s="115" t="e">
+      <c r="E34" s="115">
         <f>('Info 5'!I$4-D34)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F34" s="155" t="e">
+        <v>0.1540524901014855</v>
+      </c>
+      <c r="F34" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.1540524901014855</v>
       </c>
       <c r="G34" s="115"/>
       <c r="H34" s="115"/>
@@ -33829,13 +33947,13 @@
       <c r="D35">
         <v>0.80321621840087498</v>
       </c>
-      <c r="E35" s="115" t="e">
+      <c r="E35" s="115">
         <f>('Info 5'!I$4-D35)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F35" s="155" t="e">
+        <v>0.1705348855729524</v>
+      </c>
+      <c r="F35" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.1705348855729524</v>
       </c>
       <c r="G35" s="115"/>
       <c r="H35" s="115"/>
@@ -33855,13 +33973,13 @@
       <c r="D36">
         <v>0.51895327309119299</v>
       </c>
-      <c r="E36" s="115" t="e">
+      <c r="E36" s="115">
         <f>('Info 5'!I$4-D36)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F36" s="155" t="e">
+        <v>0.46408746961824499</v>
+      </c>
+      <c r="F36" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.46408746961824499</v>
       </c>
       <c r="G36" s="115">
         <v>250</v>
@@ -33869,17 +33987,17 @@
       <c r="H36" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I36" s="115" t="e">
+      <c r="I36" s="115">
         <f>AVERAGE(E36:E38)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J36" s="115" t="e">
+        <v>0.45798744617444642</v>
+      </c>
+      <c r="J36" s="115">
         <f>I36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K36" s="107" t="e">
+        <v>0.45798744617444642</v>
+      </c>
+      <c r="K36" s="107">
         <f>_xlfn.STDEV.P(F36:F38)</f>
-        <v>#DIV/0!</v>
+        <v>9.2514085806826764E-3</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -33895,13 +34013,13 @@
       <c r="D37">
         <v>0.51810722859230096</v>
       </c>
-      <c r="E37" s="115" t="e">
+      <c r="E37" s="115">
         <f>('Info 5'!I$4-D37)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F37" s="155" t="e">
+        <v>0.46496116263017273</v>
+      </c>
+      <c r="F37" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.46496116263017273</v>
       </c>
       <c r="G37" s="115"/>
       <c r="H37" s="115"/>
@@ -33921,13 +34039,13 @@
       <c r="D38">
         <v>0.53752027177175299</v>
       </c>
-      <c r="E38" s="115" t="e">
+      <c r="E38" s="115">
         <f>('Info 5'!I$4-D38)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F38" s="155" t="e">
+        <v>0.44491370627492161</v>
+      </c>
+      <c r="F38" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.44491370627492161</v>
       </c>
       <c r="G38" s="115"/>
       <c r="H38" s="115"/>
@@ -33947,13 +34065,13 @@
       <c r="D39" s="2">
         <v>2.6207124530528401E-2</v>
       </c>
-      <c r="E39" s="115" t="e">
+      <c r="E39" s="115">
         <f>('Info 5'!I$4-D39)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F39" s="155" t="e">
+        <v>0.97293643349134973</v>
+      </c>
+      <c r="F39" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.97293643349134973</v>
       </c>
       <c r="G39" s="115">
         <v>300</v>
@@ -33961,17 +34079,17 @@
       <c r="H39" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I39" s="115" t="e">
+      <c r="I39" s="115">
         <f>AVERAGE(E39:E43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J39" s="115" t="e">
+        <v>0.98855580773761598</v>
+      </c>
+      <c r="J39" s="115">
         <f>I39</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K39" s="107" t="e">
+        <v>0.98855580773761598</v>
+      </c>
+      <c r="K39" s="107">
         <f>_xlfn.STDEV.P(F39:F43)</f>
-        <v>#DIV/0!</v>
+        <v>1.4050319646160226E-2</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -33987,13 +34105,13 @@
       <c r="D40" s="2">
         <v>2.9203046866457701E-2</v>
       </c>
-      <c r="E40" s="115" t="e">
+      <c r="E40" s="115">
         <f>('Info 5'!I$4-D40)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F40" s="155" t="e">
+        <v>0.96984260519672993</v>
+      </c>
+      <c r="F40" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.96984260519672993</v>
       </c>
       <c r="G40" s="115"/>
       <c r="H40" s="115"/>
@@ -34013,13 +34131,13 @@
       <c r="D41">
         <v>0</v>
       </c>
-      <c r="E41" s="115" t="e">
+      <c r="E41" s="115">
         <f>('Info 5'!I$4-D41)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F41" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F41" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G41" s="115"/>
       <c r="H41" s="115"/>
@@ -34039,13 +34157,13 @@
       <c r="D42" s="2">
         <v>0</v>
       </c>
-      <c r="E42" s="115" t="e">
+      <c r="E42" s="115">
         <f>('Info 5'!I$4-D42)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F42" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F42" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G42" s="115"/>
       <c r="H42" s="115"/>
@@ -34065,13 +34183,13 @@
       <c r="D43">
         <v>0</v>
       </c>
-      <c r="E43" s="115" t="e">
+      <c r="E43" s="115">
         <f>('Info 5'!I$4-D43)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F43" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F43" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G43" s="115"/>
       <c r="H43" s="115"/>
@@ -34091,13 +34209,13 @@
       <c r="D44" s="2">
         <v>0</v>
       </c>
-      <c r="E44" s="115" t="e">
+      <c r="E44" s="115">
         <f>('Info 5'!I$4-D44)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F44" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F44" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G44" s="115">
         <v>400</v>
@@ -34105,17 +34223,17 @@
       <c r="H44" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I44" s="115" t="e">
+      <c r="I44" s="115">
         <f>AVERAGE(E44:E46)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J44" s="115" t="e">
+        <v>1</v>
+      </c>
+      <c r="J44" s="115">
         <f>I44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K44" s="107" t="e">
+        <v>1</v>
+      </c>
+      <c r="K44" s="107">
         <f>_xlfn.STDEV.P(F44:F46)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -34131,13 +34249,13 @@
       <c r="D45" s="2">
         <v>0</v>
       </c>
-      <c r="E45" s="115" t="e">
+      <c r="E45" s="115">
         <f>('Info 5'!I$4-D45)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F45" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F45" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G45" s="115"/>
       <c r="H45" s="115"/>
@@ -34157,13 +34275,13 @@
       <c r="D46" s="2">
         <v>0</v>
       </c>
-      <c r="E46" s="115" t="e">
+      <c r="E46" s="115">
         <f>('Info 5'!I$4-D46)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F46" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F46" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G46" s="115"/>
       <c r="H46" s="115"/>
@@ -34183,29 +34301,29 @@
       <c r="D47">
         <v>0.428746995855808</v>
       </c>
-      <c r="E47" s="115" t="e">
+      <c r="E47" s="115">
         <f>('Info 5'!I$4-D47)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F47" s="155" t="e">
+        <v>0.55724166441034195</v>
+      </c>
+      <c r="F47" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.55724166441034195</v>
       </c>
       <c r="G47" s="115">
         <v>250</v>
       </c>
       <c r="H47" s="115"/>
-      <c r="I47" s="115" t="e">
+      <c r="I47" s="115">
         <f>AVERAGE(E47:E50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J47" s="115" t="e">
+        <v>0.55730359308132293</v>
+      </c>
+      <c r="J47" s="115">
         <f>I47</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K47" s="107" t="e">
+        <v>0.55730359308132293</v>
+      </c>
+      <c r="K47" s="107">
         <f>_xlfn.STDEV.P(F47:F50)</f>
-        <v>#DIV/0!</v>
+        <v>2.9899941856786488E-3</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -34221,13 +34339,13 @@
       <c r="D48">
         <v>0.42630314328287799</v>
       </c>
-      <c r="E48" s="115" t="e">
+      <c r="E48" s="115">
         <f>('Info 5'!I$4-D48)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F48" s="155" t="e">
+        <v>0.55976538144643961</v>
+      </c>
+      <c r="F48" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.55976538144643961</v>
       </c>
       <c r="G48" s="115"/>
       <c r="H48" s="115"/>
@@ -34247,13 +34365,13 @@
       <c r="D49">
         <v>0.42630314328287799</v>
       </c>
-      <c r="E49" s="115" t="e">
+      <c r="E49" s="115">
         <f>('Info 5'!I$4-D49)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F49" s="155" t="e">
+        <v>0.55976538144643961</v>
+      </c>
+      <c r="F49" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.55976538144643961</v>
       </c>
       <c r="G49" s="115"/>
       <c r="H49" s="115"/>
@@ -34273,13 +34391,13 @@
       <c r="D50">
         <v>0.43339482539002</v>
       </c>
-      <c r="E50" s="115" t="e">
+      <c r="E50" s="115">
         <f>('Info 5'!I$4-D50)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F50" s="155" t="e">
+        <v>0.55244194502207067</v>
+      </c>
+      <c r="F50" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.55244194502207067</v>
       </c>
       <c r="G50" s="115"/>
       <c r="H50" s="115"/>
@@ -34299,29 +34417,29 @@
       <c r="D51" s="2">
         <v>3.1765905692637098E-2</v>
       </c>
-      <c r="E51" s="115" t="e">
+      <c r="E51" s="115">
         <f>('Info 5'!I$4-D51)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F51" s="155" t="e">
+        <v>0.96719599281413948</v>
+      </c>
+      <c r="F51" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.96719599281413948</v>
       </c>
       <c r="G51" s="115">
         <v>300</v>
       </c>
       <c r="H51" s="115"/>
-      <c r="I51" s="115" t="e">
+      <c r="I51" s="115">
         <f>AVERAGE(E51:E53)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J51" s="115" t="e">
+        <v>0.97142665254394966</v>
+      </c>
+      <c r="J51" s="115">
         <f>I51</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K51" s="107" t="e">
+        <v>0.97142665254394966</v>
+      </c>
+      <c r="K51" s="107">
         <f>_xlfn.STDEV.P(F51:F53)</f>
-        <v>#DIV/0!</v>
+        <v>1.1571778064165083E-2</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -34337,13 +34455,13 @@
       <c r="D52">
         <v>3.8878186556979999E-2</v>
       </c>
-      <c r="E52" s="115" t="e">
+      <c r="E52" s="115">
         <f>('Info 5'!I$4-D52)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F52" s="155" t="e">
+        <v>0.95985128447056967</v>
+      </c>
+      <c r="F52" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.95985128447056967</v>
       </c>
       <c r="G52" s="115"/>
       <c r="H52" s="115"/>
@@ -34363,13 +34481,13 @@
       <c r="D53" s="2">
         <v>1.23632905499218E-2</v>
       </c>
-      <c r="E53" s="115" t="e">
+      <c r="E53" s="115">
         <f>('Info 5'!I$4-D53)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F53" s="155" t="e">
+        <v>0.98723268034713962</v>
+      </c>
+      <c r="F53" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.98723268034713962</v>
       </c>
       <c r="G53" s="115"/>
       <c r="H53" s="115"/>
@@ -34389,29 +34507,29 @@
       <c r="D54">
         <v>0</v>
       </c>
-      <c r="E54" s="115" t="e">
+      <c r="E54" s="115">
         <f>('Info 5'!I$4-D54)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F54" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F54" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G54" s="115">
         <v>350</v>
       </c>
       <c r="H54" s="115"/>
-      <c r="I54" s="115" t="e">
+      <c r="I54" s="115">
         <f>AVERAGE(E54:E56)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J54" s="115" t="e">
+        <v>0.99718234712553366</v>
+      </c>
+      <c r="J54" s="115">
         <f>I54</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K54" s="107" t="e">
+        <v>0.99718234712553366</v>
+      </c>
+      <c r="K54" s="107">
         <f>_xlfn.STDEV.P(F54:F56)</f>
-        <v>#DIV/0!</v>
+        <v>3.9847629091298818E-3</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -34427,13 +34545,13 @@
       <c r="D55" s="2">
         <v>0</v>
       </c>
-      <c r="E55" s="115" t="e">
+      <c r="E55" s="115">
         <f>('Info 5'!I$4-D55)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F55" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F55" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G55" s="115"/>
       <c r="H55" s="115"/>
@@ -34453,13 +34571,13 @@
       <c r="D56" s="2">
         <v>8.1854599327851902E-3</v>
       </c>
-      <c r="E56" s="115" t="e">
+      <c r="E56" s="115">
         <f>('Info 5'!I$4-D56)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F56" s="155" t="e">
+        <v>0.99154704137660088</v>
+      </c>
+      <c r="F56" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.99154704137660088</v>
       </c>
       <c r="G56" s="115"/>
       <c r="H56" s="115"/>
@@ -34479,29 +34597,29 @@
       <c r="D57" s="2">
         <v>0</v>
       </c>
-      <c r="E57" s="115" t="e">
+      <c r="E57" s="115">
         <f>('Info 5'!I$4-D57)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F57" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F57" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G57" s="115">
         <v>400</v>
       </c>
       <c r="H57" s="115"/>
-      <c r="I57" s="115" t="e">
+      <c r="I57" s="115">
         <f>AVERAGE(E57:E59)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J57" s="115" t="e">
+        <v>1</v>
+      </c>
+      <c r="J57" s="115">
         <f>I57</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K57" s="107" t="e">
+        <v>1</v>
+      </c>
+      <c r="K57" s="107">
         <f>_xlfn.STDEV.P(F57:F59)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -34517,13 +34635,13 @@
       <c r="D58" s="2">
         <v>0</v>
       </c>
-      <c r="E58" s="115" t="e">
+      <c r="E58" s="115">
         <f>('Info 5'!I$4-D58)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F58" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F58" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G58" s="115"/>
       <c r="H58" s="115"/>
@@ -34543,13 +34661,13 @@
       <c r="D59" s="2">
         <v>0</v>
       </c>
-      <c r="E59" s="115" t="e">
+      <c r="E59" s="115">
         <f>('Info 5'!I$4-D59)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F59" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F59" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G59" s="115"/>
       <c r="H59" s="115"/>
@@ -34569,29 +34687,29 @@
       <c r="D60" s="2">
         <v>0</v>
       </c>
-      <c r="E60" s="115" t="e">
+      <c r="E60" s="115">
         <f>('Info 5'!I$4-D60)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F60" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F60" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G60" s="115">
         <v>450</v>
       </c>
       <c r="H60" s="115"/>
-      <c r="I60" s="115" t="e">
+      <c r="I60" s="115">
         <f>AVERAGE(E60:E62)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J60" s="115" t="e">
+        <v>1</v>
+      </c>
+      <c r="J60" s="115">
         <f>I60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K60" s="107" t="e">
+        <v>1</v>
+      </c>
+      <c r="K60" s="107">
         <f>_xlfn.STDEV.P(F60:F62)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -34607,13 +34725,13 @@
       <c r="D61" s="2">
         <v>0</v>
       </c>
-      <c r="E61" s="115" t="e">
+      <c r="E61" s="115">
         <f>('Info 5'!I$4-D61)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F61" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F61" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G61" s="115"/>
       <c r="H61" s="115"/>
@@ -34633,13 +34751,13 @@
       <c r="D62">
         <v>0</v>
       </c>
-      <c r="E62" s="115" t="e">
+      <c r="E62" s="115">
         <f>('Info 5'!I$4-D62)/'Info 5'!I$4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F62" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F62" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G62" s="115"/>
       <c r="H62" s="115"/>
@@ -34673,13 +34791,13 @@
       <c r="D64">
         <v>0.98</v>
       </c>
-      <c r="E64" s="115" t="e">
+      <c r="E64" s="115">
         <f>('Info 5'!I$5-D64)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F64" s="155" t="e">
+        <v>-2.4770642201829654E-3</v>
+      </c>
+      <c r="F64" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>-2.4770642201829654E-3</v>
       </c>
       <c r="G64" s="115">
         <v>150</v>
@@ -34687,17 +34805,17 @@
       <c r="H64" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I64" s="115" t="e">
+      <c r="I64" s="115">
         <f>AVERAGE(E64:E66)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J64" s="115" t="e">
+        <v>-2.4770642201829654E-3</v>
+      </c>
+      <c r="J64" s="115">
         <f>I64</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K64" s="107" t="e">
+        <v>-2.4770642201829654E-3</v>
+      </c>
+      <c r="K64" s="107">
         <f>_xlfn.STDEV.P(F64:F66)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -34713,13 +34831,13 @@
       <c r="D65">
         <v>0.98</v>
       </c>
-      <c r="E65" s="115" t="e">
+      <c r="E65" s="115">
         <f>('Info 5'!I$5-D65)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F65" s="155" t="e">
+        <v>-2.4770642201829654E-3</v>
+      </c>
+      <c r="F65" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>-2.4770642201829654E-3</v>
       </c>
       <c r="G65" s="115"/>
       <c r="H65" s="115"/>
@@ -34739,13 +34857,13 @@
       <c r="D66">
         <v>0.98</v>
       </c>
-      <c r="E66" s="115" t="e">
+      <c r="E66" s="115">
         <f>('Info 5'!I$5-D66)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F66" s="155" t="e">
+        <v>-2.4770642201829654E-3</v>
+      </c>
+      <c r="F66" s="155">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>-2.4770642201829654E-3</v>
       </c>
       <c r="G66" s="115"/>
       <c r="H66" s="115"/>
@@ -34765,13 +34883,13 @@
       <c r="D67">
         <v>0.79111844826315403</v>
       </c>
-      <c r="E67" s="115" t="e">
+      <c r="E67" s="115">
         <f>('Info 5'!I$5-D67)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F67" s="155" t="e">
+        <v>0.19073663319870066</v>
+      </c>
+      <c r="F67" s="155">
         <f t="shared" ref="F67:F130" si="1">E67</f>
-        <v>#DIV/0!</v>
+        <v>0.19073663319870066</v>
       </c>
       <c r="G67" s="115">
         <v>250</v>
@@ -34779,17 +34897,17 @@
       <c r="H67" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I67" s="115" t="e">
+      <c r="I67" s="115">
         <f>AVERAGE(E67:E69)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J67" s="115" t="e">
+        <v>0.17804848493952721</v>
+      </c>
+      <c r="J67" s="115">
         <f>I67</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K67" s="107" t="e">
+        <v>0.17804848493952721</v>
+      </c>
+      <c r="K67" s="107">
         <f>_xlfn.STDEV.P(F67:F69)</f>
-        <v>#DIV/0!</v>
+        <v>9.0641552244555886E-3</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -34805,13 +34923,13 @@
       <c r="D68">
         <v>0.81126855502866901</v>
       </c>
-      <c r="E68" s="115" t="e">
+      <c r="E68" s="115">
         <f>('Info 5'!I$5-D68)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F68" s="155" t="e">
+        <v>0.17012436802113257</v>
+      </c>
+      <c r="F68" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.17012436802113257</v>
       </c>
       <c r="G68" s="115"/>
       <c r="H68" s="115"/>
@@ -34831,13 +34949,13 @@
       <c r="D69">
         <v>0.80817932338777099</v>
       </c>
-      <c r="E69" s="115" t="e">
+      <c r="E69" s="115">
         <f>('Info 5'!I$5-D69)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F69" s="155" t="e">
+        <v>0.17328445359874844</v>
+      </c>
+      <c r="F69" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.17328445359874844</v>
       </c>
       <c r="G69" s="115"/>
       <c r="H69" s="115"/>
@@ -34857,13 +34975,13 @@
       <c r="D70">
         <v>0.28687991593531498</v>
       </c>
-      <c r="E70" s="115" t="e">
+      <c r="E70" s="115">
         <f>('Info 5'!I$5-D70)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F70" s="155" t="e">
+        <v>0.70654026947901283</v>
+      </c>
+      <c r="F70" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.70654026947901283</v>
       </c>
       <c r="G70" s="115">
         <v>300</v>
@@ -34871,17 +34989,17 @@
       <c r="H70" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I70" s="115" t="e">
+      <c r="I70" s="115">
         <f>AVERAGE(E70:E74)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J70" s="115" t="e">
+        <v>0.8154829905041856</v>
+      </c>
+      <c r="J70" s="115">
         <f>I70</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K70" s="107" t="e">
+        <v>0.8154829905041856</v>
+      </c>
+      <c r="K70" s="107">
         <f>_xlfn.STDEV.P(F70:F74)</f>
-        <v>#DIV/0!</v>
+        <v>9.2429605711833146E-2</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -34897,13 +35015,13 @@
       <c r="D71">
         <v>0.29410557880847998</v>
       </c>
-      <c r="E71" s="115" t="e">
+      <c r="E71" s="115">
         <f>('Info 5'!I$5-D71)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F71" s="155" t="e">
+        <v>0.69914888039316059</v>
+      </c>
+      <c r="F71" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.69914888039316059</v>
       </c>
       <c r="G71" s="115"/>
       <c r="H71" s="115"/>
@@ -34923,13 +35041,13 @@
       <c r="D72">
         <v>0.12139215706800099</v>
       </c>
-      <c r="E72" s="115" t="e">
+      <c r="E72" s="115">
         <f>('Info 5'!I$5-D72)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F72" s="155" t="e">
+        <v>0.87582361914603579</v>
+      </c>
+      <c r="F72" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.87582361914603579</v>
       </c>
       <c r="G72" s="115"/>
       <c r="H72" s="115"/>
@@ -34949,13 +35067,13 @@
       <c r="D73">
         <v>0.105587524556167</v>
       </c>
-      <c r="E73" s="115" t="e">
+      <c r="E73" s="115">
         <f>('Info 5'!I$5-D73)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F73" s="155" t="e">
+        <v>0.89199074322924199</v>
+      </c>
+      <c r="F73" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.89199074322924199</v>
       </c>
       <c r="G73" s="115"/>
       <c r="H73" s="115"/>
@@ -34975,13 +35093,13 @@
       <c r="D74">
         <v>9.3934107714717996E-2</v>
       </c>
-      <c r="E74" s="115" t="e">
+      <c r="E74" s="115">
         <f>('Info 5'!I$5-D74)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F74" s="155" t="e">
+        <v>0.90391144027347659</v>
+      </c>
+      <c r="F74" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.90391144027347659</v>
       </c>
       <c r="G74" s="115"/>
       <c r="H74" s="115"/>
@@ -35001,13 +35119,13 @@
       <c r="D75">
         <v>0.103244401158383</v>
       </c>
-      <c r="E75" s="115" t="e">
+      <c r="E75" s="115">
         <f>('Info 5'!I$5-D75)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F75" s="155" t="e">
+        <v>0.89438760798936057</v>
+      </c>
+      <c r="F75" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.89438760798936057</v>
       </c>
       <c r="G75" s="115">
         <v>400</v>
@@ -35015,17 +35133,17 @@
       <c r="H75" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I75" s="115" t="e">
+      <c r="I75" s="115">
         <f>AVERAGE(E75:E77)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J75" s="115" t="e">
+        <v>0.93813490393135501</v>
+      </c>
+      <c r="J75" s="115">
         <f>I75</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K75" s="107" t="e">
+        <v>0.93813490393135501</v>
+      </c>
+      <c r="K75" s="107">
         <f>_xlfn.STDEV.P(F75:F77)</f>
-        <v>#DIV/0!</v>
+        <v>3.1937691324337346E-2</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -35041,13 +35159,13 @@
       <c r="D76" s="2">
         <v>4.8605706312992901E-2</v>
       </c>
-      <c r="E76" s="115" t="e">
+      <c r="E76" s="115">
         <f>('Info 5'!I$5-D76)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F76" s="155" t="e">
+        <v>0.95027948390918626</v>
+      </c>
+      <c r="F76" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.95027948390918626</v>
       </c>
       <c r="G76" s="115"/>
       <c r="H76" s="115"/>
@@ -35067,13 +35185,13 @@
       <c r="D77" s="2">
         <v>2.95838514025876E-2</v>
       </c>
-      <c r="E77" s="115" t="e">
+      <c r="E77" s="115">
         <f>('Info 5'!I$5-D77)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F77" s="155" t="e">
+        <v>0.96973761989551821</v>
+      </c>
+      <c r="F77" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.96973761989551821</v>
       </c>
       <c r="G77" s="115"/>
       <c r="H77" s="115"/>
@@ -35093,29 +35211,29 @@
       <c r="D78">
         <v>0.71808511798277697</v>
       </c>
-      <c r="E78" s="115" t="e">
+      <c r="E78" s="115">
         <f>('Info 5'!I$5-D78)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F78" s="155" t="e">
+        <v>0.26544503986165513</v>
+      </c>
+      <c r="F78" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.26544503986165513</v>
       </c>
       <c r="G78" s="115">
         <v>250</v>
       </c>
       <c r="H78" s="115"/>
-      <c r="I78" s="115" t="e">
+      <c r="I78" s="115">
         <f>AVERAGE(E78:E81)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J78" s="115" t="e">
+        <v>0.30453863787194396</v>
+      </c>
+      <c r="J78" s="115">
         <f>I78</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K78" s="107" t="e">
+        <v>0.30453863787194396</v>
+      </c>
+      <c r="K78" s="107">
         <f>_xlfn.STDEV.P(F78:F81)</f>
-        <v>#DIV/0!</v>
+        <v>2.257749777329069E-2</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -35131,13 +35249,13 @@
       <c r="D79">
         <v>0.66757125033892295</v>
       </c>
-      <c r="E79" s="115" t="e">
+      <c r="E79" s="115">
         <f>('Info 5'!I$5-D79)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F79" s="155" t="e">
+        <v>0.31711748245146909</v>
+      </c>
+      <c r="F79" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.31711748245146909</v>
       </c>
       <c r="G79" s="115"/>
       <c r="H79" s="115"/>
@@ -35157,13 +35275,13 @@
       <c r="D80">
         <v>0.66757125033892295</v>
       </c>
-      <c r="E80" s="115" t="e">
+      <c r="E80" s="115">
         <f>('Info 5'!I$5-D80)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F80" s="155" t="e">
+        <v>0.31711748245146909</v>
+      </c>
+      <c r="F80" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.31711748245146909</v>
       </c>
       <c r="G80" s="115"/>
       <c r="H80" s="115"/>
@@ -35183,13 +35301,13 @@
       <c r="D81">
         <v>0.66624461351724795</v>
       </c>
-      <c r="E81" s="115" t="e">
+      <c r="E81" s="115">
         <f>('Info 5'!I$5-D81)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F81" s="155" t="e">
+        <v>0.31847454672318248</v>
+      </c>
+      <c r="F81" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.31847454672318248</v>
       </c>
       <c r="G81" s="115"/>
       <c r="H81" s="115"/>
@@ -35209,29 +35327,29 @@
       <c r="D82">
         <v>0.176488600476404</v>
       </c>
-      <c r="E82" s="115" t="e">
+      <c r="E82" s="115">
         <f>('Info 5'!I$5-D82)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F82" s="155" t="e">
+        <v>0.81946349584294464</v>
+      </c>
+      <c r="F82" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.81946349584294464</v>
       </c>
       <c r="G82" s="115">
         <v>300</v>
       </c>
       <c r="H82" s="115"/>
-      <c r="I82" s="115" t="e">
+      <c r="I82" s="115">
         <f>AVERAGE(E82:E84)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J82" s="115" t="e">
+        <v>0.81891596388335552</v>
+      </c>
+      <c r="J82" s="115">
         <f>I82</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K82" s="107" t="e">
+        <v>0.81891596388335552</v>
+      </c>
+      <c r="K82" s="107">
         <f>_xlfn.STDEV.P(F82:F84)</f>
-        <v>#DIV/0!</v>
+        <v>3.2096858101791526E-2</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -35247,13 +35365,13 @@
       <c r="D83">
         <v>0.21571774968882099</v>
       </c>
-      <c r="E83" s="115" t="e">
+      <c r="E83" s="115">
         <f>('Info 5'!I$5-D83)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F83" s="155" t="e">
+        <v>0.77933459550180251</v>
+      </c>
+      <c r="F83" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.77933459550180251</v>
       </c>
       <c r="G83" s="115"/>
       <c r="H83" s="115"/>
@@ -35273,13 +35391,13 @@
       <c r="D84">
         <v>0.13886521763874601</v>
       </c>
-      <c r="E84" s="115" t="e">
+      <c r="E84" s="115">
         <f>('Info 5'!I$5-D84)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F84" s="155" t="e">
+        <v>0.85794980030531953</v>
+      </c>
+      <c r="F84" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.85794980030531953</v>
       </c>
       <c r="G84" s="115"/>
       <c r="H84" s="115"/>
@@ -35299,29 +35417,29 @@
       <c r="D85" s="2">
         <v>5.2747447287354199E-2</v>
       </c>
-      <c r="E85" s="115" t="e">
+      <c r="E85" s="115">
         <f>('Info 5'!I$5-D85)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F85" s="155" t="e">
+        <v>0.94604274887577988</v>
+      </c>
+      <c r="F85" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.94604274887577988</v>
       </c>
       <c r="G85" s="115">
         <v>350</v>
       </c>
       <c r="H85" s="115"/>
-      <c r="I85" s="115" t="e">
+      <c r="I85" s="115">
         <f>AVERAGE(E85:E87)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J85" s="115" t="e">
+        <v>0.92711166311218385</v>
+      </c>
+      <c r="J85" s="115">
         <f>I85</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K85" s="107" t="e">
+        <v>0.92711166311218385</v>
+      </c>
+      <c r="K85" s="107">
         <f>_xlfn.STDEV.P(F85:F87)</f>
-        <v>#DIV/0!</v>
+        <v>2.3829095147899368E-2</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -35337,13 +35455,13 @@
       <c r="D86" s="2">
         <v>5.6904393073744799E-2</v>
       </c>
-      <c r="E86" s="115" t="e">
+      <c r="E86" s="115">
         <f>('Info 5'!I$5-D86)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F86" s="155" t="e">
+        <v>0.94179046029612346</v>
+      </c>
+      <c r="F86" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.94179046029612346</v>
       </c>
       <c r="G86" s="115"/>
       <c r="H86" s="115"/>
@@ -35363,13 +35481,13 @@
       <c r="D87">
         <v>0.104110367372676</v>
       </c>
-      <c r="E87" s="115" t="e">
+      <c r="E87" s="115">
         <f>('Info 5'!I$5-D87)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F87" s="155" t="e">
+        <v>0.89350178016464799</v>
+      </c>
+      <c r="F87" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.89350178016464799</v>
       </c>
       <c r="G87" s="115"/>
       <c r="H87" s="115"/>
@@ -35389,29 +35507,29 @@
       <c r="D88">
         <v>0.106422814977936</v>
       </c>
-      <c r="E88" s="115" t="e">
+      <c r="E88" s="115">
         <f>('Info 5'!I$5-D88)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F88" s="155" t="e">
+        <v>0.89113629477027645</v>
+      </c>
+      <c r="F88" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.89113629477027645</v>
       </c>
       <c r="G88" s="115">
         <v>400</v>
       </c>
       <c r="H88" s="115"/>
-      <c r="I88" s="115" t="e">
+      <c r="I88" s="115">
         <f>AVERAGE(E88:E90)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J88" s="115" t="e">
+        <v>0.9072640463440852</v>
+      </c>
+      <c r="J88" s="115">
         <f>I88</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K88" s="107" t="e">
+        <v>0.9072640463440852</v>
+      </c>
+      <c r="K88" s="107">
         <f>_xlfn.STDEV.P(F88:F90)</f>
-        <v>#DIV/0!</v>
+        <v>1.3543285845548198E-2</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -35427,13 +35545,13 @@
       <c r="D89" s="2">
         <v>9.1520203009964399E-2</v>
       </c>
-      <c r="E89" s="115" t="e">
+      <c r="E89" s="115">
         <f>('Info 5'!I$5-D89)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F89" s="155" t="e">
+        <v>0.90638070976503637</v>
+      </c>
+      <c r="F89" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.90638070976503637</v>
       </c>
       <c r="G89" s="115"/>
       <c r="H89" s="115"/>
@@ -35453,13 +35571,13 @@
       <c r="D90" s="2">
         <v>7.4026998563526597E-2</v>
       </c>
-      <c r="E90" s="115" t="e">
+      <c r="E90" s="115">
         <f>('Info 5'!I$5-D90)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F90" s="155" t="e">
+        <v>0.9242751344969431</v>
+      </c>
+      <c r="F90" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.9242751344969431</v>
       </c>
       <c r="G90" s="115"/>
       <c r="H90" s="115"/>
@@ -35479,29 +35597,29 @@
       <c r="D91" s="2">
         <v>9.31380004829898E-2</v>
       </c>
-      <c r="E91" s="115" t="e">
+      <c r="E91" s="115">
         <f>('Info 5'!I$5-D91)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F91" s="155" t="e">
+        <v>0.90472580684538206</v>
+      </c>
+      <c r="F91" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.90472580684538206</v>
       </c>
       <c r="G91" s="115">
         <v>450</v>
       </c>
       <c r="H91" s="115"/>
-      <c r="I91" s="115" t="e">
+      <c r="I91" s="115">
         <f>AVERAGE(E91:E93)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J91" s="115" t="e">
+        <v>0.92724376979658973</v>
+      </c>
+      <c r="J91" s="115">
         <f>I91</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K91" s="107" t="e">
+        <v>0.92724376979658973</v>
+      </c>
+      <c r="K91" s="107">
         <f>_xlfn.STDEV.P(F91:F93)</f>
-        <v>#DIV/0!</v>
+        <v>1.6107115880675545E-2</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -35517,13 +35635,13 @@
       <c r="D92" s="2">
         <v>6.3029007562272504E-2</v>
       </c>
-      <c r="E92" s="115" t="e">
+      <c r="E92" s="115">
         <f>('Info 5'!I$5-D92)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F92" s="155" t="e">
+        <v>0.93552537299822591</v>
+      </c>
+      <c r="F92" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.93552537299822591</v>
       </c>
       <c r="G92" s="115"/>
       <c r="H92" s="115"/>
@@ -35543,13 +35661,13 @@
       <c r="D93" s="2">
         <v>5.7207765735142899E-2</v>
       </c>
-      <c r="E93" s="115" t="e">
+      <c r="E93" s="115">
         <f>('Info 5'!I$5-D93)/'Info 5'!I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F93" s="155" t="e">
+        <v>0.94148012954616123</v>
+      </c>
+      <c r="F93" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.94148012954616123</v>
       </c>
       <c r="G93" s="115"/>
       <c r="H93" s="115"/>
@@ -36493,13 +36611,13 @@
       <c r="D126">
         <v>0.84896053098662005</v>
       </c>
-      <c r="E126" s="115" t="e">
+      <c r="E126" s="115">
         <f>('Info 5'!I$7-D126)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F126" s="155" t="e">
+        <v>0.16041502097665716</v>
+      </c>
+      <c r="F126" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.16041502097665716</v>
       </c>
       <c r="G126" s="115">
         <v>150</v>
@@ -36507,17 +36625,17 @@
       <c r="H126" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I126" s="115" t="e">
+      <c r="I126" s="115">
         <f>AVERAGE(E126:E128)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J126" s="115" t="e">
+        <v>0.17010401323150406</v>
+      </c>
+      <c r="J126" s="115">
         <f>I126</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K126" s="107" t="e">
+        <v>0.17010401323150406</v>
+      </c>
+      <c r="K126" s="107">
         <f>_xlfn.STDEV.P(F126:F128)</f>
-        <v>#DIV/0!</v>
+        <v>7.5161795950785659E-3</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
@@ -36533,13 +36651,13 @@
       <c r="D127">
         <v>0.83809278747008198</v>
       </c>
-      <c r="E127" s="115" t="e">
+      <c r="E127" s="115">
         <f>('Info 5'!I$7-D127)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F127" s="155" t="e">
+        <v>0.17116274584645735</v>
+      </c>
+      <c r="F127" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.17116274584645735</v>
       </c>
       <c r="G127" s="115"/>
       <c r="H127" s="115"/>
@@ -36559,13 +36677,13 @@
       <c r="D128">
         <v>0.83043671004603103</v>
       </c>
-      <c r="E128" s="115" t="e">
+      <c r="E128" s="115">
         <f>('Info 5'!I$7-D128)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F128" s="155" t="e">
+        <v>0.1787342728713977</v>
+      </c>
+      <c r="F128" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.1787342728713977</v>
       </c>
       <c r="G128" s="115"/>
       <c r="H128" s="115"/>
@@ -36585,13 +36703,13 @@
       <c r="D129">
         <v>0.72922872198730804</v>
       </c>
-      <c r="E129" s="115" t="e">
+      <c r="E129" s="115">
         <f>('Info 5'!I$7-D129)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F129" s="155" t="e">
+        <v>0.27882456379755727</v>
+      </c>
+      <c r="F129" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.27882456379755727</v>
       </c>
       <c r="G129" s="115">
         <v>250</v>
@@ -36599,17 +36717,17 @@
       <c r="H129" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I129" s="115" t="e">
+      <c r="I129" s="115">
         <f>AVERAGE(E129:E131)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J129" s="115" t="e">
+        <v>0.27048952362705209</v>
+      </c>
+      <c r="J129" s="115">
         <f>I129</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K129" s="107" t="e">
+        <v>0.27048952362705209</v>
+      </c>
+      <c r="K129" s="107">
         <f>_xlfn.STDEV.P(F129:F131)</f>
-        <v>#DIV/0!</v>
+        <v>1.4862712412737041E-2</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
@@ -36625,13 +36743,13 @@
       <c r="D130">
         <v>0.72497364593565705</v>
       </c>
-      <c r="E130" s="115" t="e">
+      <c r="E130" s="115">
         <f>('Info 5'!I$7-D130)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F130" s="155" t="e">
+        <v>0.28303264863445343</v>
+      </c>
+      <c r="F130" s="155">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.28303264863445343</v>
       </c>
       <c r="G130" s="115"/>
       <c r="H130" s="115"/>
@@ -36651,13 +36769,13 @@
       <c r="D131">
         <v>0.75876814794661795</v>
       </c>
-      <c r="E131" s="115" t="e">
+      <c r="E131" s="115">
         <f>('Info 5'!I$7-D131)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F131" s="155" t="e">
+        <v>0.2496113584491455</v>
+      </c>
+      <c r="F131" s="155">
         <f t="shared" ref="F131:F194" si="2">E131</f>
-        <v>#DIV/0!</v>
+        <v>0.2496113584491455</v>
       </c>
       <c r="G131" s="115"/>
       <c r="H131" s="115"/>
@@ -36677,13 +36795,13 @@
       <c r="D132">
         <v>0.43077542987492201</v>
       </c>
-      <c r="E132" s="115" t="e">
+      <c r="E132" s="115">
         <f>('Info 5'!I$7-D132)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F132" s="155" t="e">
+        <v>0.57398186717232913</v>
+      </c>
+      <c r="F132" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.57398186717232913</v>
       </c>
       <c r="G132" s="115">
         <v>300</v>
@@ -36691,17 +36809,17 @@
       <c r="H132" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I132" s="115" t="e">
+      <c r="I132" s="115">
         <f>AVERAGE(E132:E136)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J132" s="115" t="e">
+        <v>0.83113037349894814</v>
+      </c>
+      <c r="J132" s="115">
         <f>I132</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K132" s="107" t="e">
+        <v>0.83113037349894814</v>
+      </c>
+      <c r="K132" s="107">
         <f>_xlfn.STDEV.P(F132:F136)</f>
-        <v>#DIV/0!</v>
+        <v>0.20683649791813932</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
@@ -36717,13 +36835,13 @@
       <c r="D133">
         <v>0.42300144419811497</v>
       </c>
-      <c r="E133" s="115" t="e">
+      <c r="E133" s="115">
         <f>('Info 5'!I$7-D133)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F133" s="155" t="e">
+        <v>0.58167000032241156</v>
+      </c>
+      <c r="F133" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.58167000032241156</v>
       </c>
       <c r="G133" s="115"/>
       <c r="H133" s="115"/>
@@ -36743,13 +36861,13 @@
       <c r="D134">
         <v>0</v>
       </c>
-      <c r="E134" s="115" t="e">
+      <c r="E134" s="115">
         <f>('Info 5'!I$7-D134)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F134" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F134" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G134" s="115"/>
       <c r="H134" s="115"/>
@@ -36769,13 +36887,13 @@
       <c r="D135">
         <v>0</v>
       </c>
-      <c r="E135" s="115" t="e">
+      <c r="E135" s="115">
         <f>('Info 5'!I$7-D135)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F135" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F135" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G135" s="115"/>
       <c r="H135" s="115"/>
@@ -36795,13 +36913,13 @@
       <c r="D136">
         <v>0</v>
       </c>
-      <c r="E136" s="115" t="e">
+      <c r="E136" s="115">
         <f>('Info 5'!I$7-D136)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F136" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F136" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G136" s="115"/>
       <c r="H136" s="115"/>
@@ -36821,13 +36939,13 @@
       <c r="D137">
         <v>0</v>
       </c>
-      <c r="E137" s="115" t="e">
+      <c r="E137" s="115">
         <f>('Info 5'!I$7-D137)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F137" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F137" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G137" s="115">
         <v>400</v>
@@ -36835,17 +36953,17 @@
       <c r="H137" s="115" t="s">
         <v>1538</v>
       </c>
-      <c r="I137" s="115" t="e">
+      <c r="I137" s="115">
         <f>AVERAGE(E137:E139)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J137" s="115" t="e">
+        <v>1</v>
+      </c>
+      <c r="J137" s="115">
         <f>I137</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K137" s="107" t="e">
+        <v>1</v>
+      </c>
+      <c r="K137" s="107">
         <f>_xlfn.STDEV.P(F137:F139)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
@@ -36861,13 +36979,13 @@
       <c r="D138">
         <v>0</v>
       </c>
-      <c r="E138" s="115" t="e">
+      <c r="E138" s="115">
         <f>('Info 5'!I$7-D138)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F138" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F138" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G138" s="115"/>
       <c r="H138" s="115"/>
@@ -36887,13 +37005,13 @@
       <c r="D139">
         <v>0</v>
       </c>
-      <c r="E139" s="115" t="e">
+      <c r="E139" s="115">
         <f>('Info 5'!I$7-D139)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F139" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F139" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G139" s="115"/>
       <c r="H139" s="115"/>
@@ -36913,29 +37031,29 @@
       <c r="D140">
         <v>0.64771928243263799</v>
       </c>
-      <c r="E140" s="115" t="e">
+      <c r="E140" s="115">
         <f>('Info 5'!I$7-D140)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F140" s="155" t="e">
+        <v>0.35943384844731752</v>
+      </c>
+      <c r="F140" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.35943384844731752</v>
       </c>
       <c r="G140" s="115">
         <v>250</v>
       </c>
       <c r="H140" s="115"/>
-      <c r="I140" s="115" t="e">
+      <c r="I140" s="115">
         <f>AVERAGE(E140:E143)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J140" s="115" t="e">
+        <v>0.38410957541292601</v>
+      </c>
+      <c r="J140" s="115">
         <f>I140</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K140" s="107" t="e">
+        <v>0.38410957541292601</v>
+      </c>
+      <c r="K140" s="107">
         <f>_xlfn.STDEV.P(F140:F143)</f>
-        <v>#DIV/0!</v>
+        <v>1.4294366274479442E-2</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
@@ -36951,13 +37069,13 @@
       <c r="D141">
         <v>0.61348629400659704</v>
       </c>
-      <c r="E141" s="115" t="e">
+      <c r="E141" s="115">
         <f>('Info 5'!I$7-D141)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F141" s="155" t="e">
+        <v>0.39328878259388139</v>
+      </c>
+      <c r="F141" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.39328878259388139</v>
       </c>
       <c r="G141" s="115"/>
       <c r="H141" s="115"/>
@@ -36977,13 +37095,13 @@
       <c r="D142">
         <v>0.61348629400659704</v>
       </c>
-      <c r="E142" s="115" t="e">
+      <c r="E142" s="115">
         <f>('Info 5'!I$7-D142)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F142" s="155" t="e">
+        <v>0.39328878259388139</v>
+      </c>
+      <c r="F142" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.39328878259388139</v>
       </c>
       <c r="G142" s="115"/>
       <c r="H142" s="115"/>
@@ -37003,13 +37121,13 @@
       <c r="D143">
         <v>0.61638014704189403</v>
       </c>
-      <c r="E143" s="115" t="e">
+      <c r="E143" s="115">
         <f>('Info 5'!I$7-D143)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F143" s="155" t="e">
+        <v>0.39042688801662367</v>
+      </c>
+      <c r="F143" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.39042688801662367</v>
       </c>
       <c r="G143" s="115"/>
       <c r="H143" s="115"/>
@@ -37029,29 +37147,29 @@
       <c r="D144">
         <v>0.24434153553437901</v>
       </c>
-      <c r="E144" s="115" t="e">
+      <c r="E144" s="115">
         <f>('Info 5'!I$7-D144)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F144" s="155" t="e">
+        <v>0.75835686642846278</v>
+      </c>
+      <c r="F144" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.75835686642846278</v>
       </c>
       <c r="G144" s="115">
         <v>300</v>
       </c>
       <c r="H144" s="115"/>
-      <c r="I144" s="115" t="e">
+      <c r="I144" s="115">
         <f>AVERAGE(E144:E146)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J144" s="115" t="e">
+        <v>0.72958675893083791</v>
+      </c>
+      <c r="J144" s="115">
         <f>I144</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K144" s="107" t="e">
+        <v>0.72958675893083791</v>
+      </c>
+      <c r="K144" s="107">
         <f>_xlfn.STDEV.P(F144:F146)</f>
-        <v>#DIV/0!</v>
+        <v>2.3981633326539423E-2</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
@@ -37067,13 +37185,13 @@
       <c r="D145">
         <v>0.303705056157348</v>
       </c>
-      <c r="E145" s="115" t="e">
+      <c r="E145" s="115">
         <f>('Info 5'!I$7-D145)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F145" s="155" t="e">
+        <v>0.699648930785018</v>
+      </c>
+      <c r="F145" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.699648930785018</v>
       </c>
       <c r="G145" s="115"/>
       <c r="H145" s="115"/>
@@ -37093,13 +37211,13 @@
       <c r="D146">
         <v>0.27225215516391199</v>
       </c>
-      <c r="E146" s="115" t="e">
+      <c r="E146" s="115">
         <f>('Info 5'!I$7-D146)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F146" s="155" t="e">
+        <v>0.73075447957903306</v>
+      </c>
+      <c r="F146" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.73075447957903306</v>
       </c>
       <c r="G146" s="115"/>
       <c r="H146" s="115"/>
@@ -37119,29 +37237,29 @@
       <c r="D147">
         <v>0</v>
       </c>
-      <c r="E147" s="115" t="e">
+      <c r="E147" s="115">
         <f>('Info 5'!I$7-D147)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F147" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F147" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G147" s="115">
         <v>350</v>
       </c>
       <c r="H147" s="115"/>
-      <c r="I147" s="115" t="e">
+      <c r="I147" s="115">
         <f>AVERAGE(E147:E149)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J147" s="115" t="e">
+        <v>1</v>
+      </c>
+      <c r="J147" s="115">
         <f>I147</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K147" s="107" t="e">
+        <v>1</v>
+      </c>
+      <c r="K147" s="107">
         <f>_xlfn.STDEV.P(F147:F149)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
@@ -37157,13 +37275,13 @@
       <c r="D148">
         <v>0</v>
       </c>
-      <c r="E148" s="115" t="e">
+      <c r="E148" s="115">
         <f>('Info 5'!I$7-D148)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F148" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F148" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G148" s="115"/>
       <c r="H148" s="115"/>
@@ -37183,13 +37301,13 @@
       <c r="D149" s="2">
         <v>0</v>
       </c>
-      <c r="E149" s="115" t="e">
+      <c r="E149" s="115">
         <f>('Info 5'!I$7-D149)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F149" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F149" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G149" s="115"/>
       <c r="H149" s="115"/>
@@ -37209,29 +37327,29 @@
       <c r="D150">
         <v>0</v>
       </c>
-      <c r="E150" s="115" t="e">
+      <c r="E150" s="115">
         <f>('Info 5'!I$7-D150)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F150" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F150" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G150" s="115">
         <v>400</v>
       </c>
       <c r="H150" s="115"/>
-      <c r="I150" s="115" t="e">
+      <c r="I150" s="115">
         <f>AVERAGE(E150:E152)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J150" s="115" t="e">
+        <v>1</v>
+      </c>
+      <c r="J150" s="115">
         <f>I150</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K150" s="107" t="e">
+        <v>1</v>
+      </c>
+      <c r="K150" s="107">
         <f>_xlfn.STDEV.P(F150:F152)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
@@ -37247,13 +37365,13 @@
       <c r="D151">
         <v>0</v>
       </c>
-      <c r="E151" s="115" t="e">
+      <c r="E151" s="115">
         <f>('Info 5'!I$7-D151)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F151" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F151" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G151" s="115"/>
       <c r="H151" s="115"/>
@@ -37273,13 +37391,13 @@
       <c r="D152">
         <v>0</v>
       </c>
-      <c r="E152" s="115" t="e">
+      <c r="E152" s="115">
         <f>('Info 5'!I$7-D152)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F152" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F152" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G152" s="115"/>
       <c r="H152" s="115"/>
@@ -37299,29 +37417,29 @@
       <c r="D153">
         <v>0</v>
       </c>
-      <c r="E153" s="115" t="e">
+      <c r="E153" s="115">
         <f>('Info 5'!I$7-D153)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F153" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F153" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G153" s="115">
         <v>450</v>
       </c>
       <c r="H153" s="115"/>
-      <c r="I153" s="115" t="e">
+      <c r="I153" s="115">
         <f>AVERAGE(E153:E155)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J153" s="115" t="e">
+        <v>1</v>
+      </c>
+      <c r="J153" s="115">
         <f>I153</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K153" s="107" t="e">
+        <v>1</v>
+      </c>
+      <c r="K153" s="107">
         <f>_xlfn.STDEV.P(F153:F155)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
@@ -37337,13 +37455,13 @@
       <c r="D154">
         <v>0</v>
       </c>
-      <c r="E154" s="115" t="e">
+      <c r="E154" s="115">
         <f>('Info 5'!I$7-D154)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F154" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F154" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G154" s="115"/>
       <c r="H154" s="115"/>
@@ -37363,13 +37481,13 @@
       <c r="D155">
         <v>0</v>
       </c>
-      <c r="E155" s="115" t="e">
+      <c r="E155" s="115">
         <f>('Info 5'!I$7-D155)/'Info 5'!I$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F155" s="155" t="e">
+        <v>1</v>
+      </c>
+      <c r="F155" s="155">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G155" s="115"/>
       <c r="H155" s="115"/>
@@ -45634,7 +45752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -46378,7 +46496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N386"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -55082,7 +55200,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>